<commit_message>
Added the excel sheet as well
</commit_message>
<xml_diff>
--- a/Dance Competition Sheet.xlsx
+++ b/Dance Competition Sheet.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adammcpherson/Documents/DM1/TA/Dance Competion/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adammcpherson/Documents/DM1/TA/DanceCompetition/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49463D87-00F7-F841-A266-735D529FD86F}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F834A67A-32F4-C34A-BFB7-B81F3CEB908C}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{D9D28937-1BC5-C94D-91B6-1BFC68270A7E}"/>
   </bookViews>
@@ -4380,8 +4380,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{728F71C9-42E1-6448-AE41-E1190B29DDE7}">
   <dimension ref="A2:AF61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="S27" sqref="S27"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="125" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4533,11 +4533,21 @@
       <c r="A27" s="5">
         <v>111</v>
       </c>
-      <c r="B27" s="6"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="7"/>
-      <c r="E27" s="7"/>
-      <c r="F27" s="7"/>
+      <c r="B27" s="6">
+        <v>7</v>
+      </c>
+      <c r="C27" s="7">
+        <v>7</v>
+      </c>
+      <c r="D27" s="7">
+        <v>7</v>
+      </c>
+      <c r="E27" s="7">
+        <v>7</v>
+      </c>
+      <c r="F27" s="7">
+        <v>7</v>
+      </c>
       <c r="G27" s="6"/>
       <c r="H27" s="7"/>
       <c r="I27" s="7"/>
@@ -4568,11 +4578,11 @@
       </c>
       <c r="Q27" s="57">
         <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=7")</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="R27" s="57">
         <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=8")</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="S27" s="57">
         <f>SUMIF(Table5[[#This Row],[A]:[E]],"&lt;=FILL THIS IN")</f>
@@ -4626,11 +4636,21 @@
       <c r="A28" s="9">
         <v>112</v>
       </c>
-      <c r="B28" s="10"/>
-      <c r="C28" s="10"/>
-      <c r="D28" s="10"/>
-      <c r="E28" s="10"/>
-      <c r="F28" s="10"/>
+      <c r="B28" s="10">
+        <v>4</v>
+      </c>
+      <c r="C28" s="10">
+        <v>6</v>
+      </c>
+      <c r="D28" s="10">
+        <v>3</v>
+      </c>
+      <c r="E28" s="10">
+        <v>6</v>
+      </c>
+      <c r="F28" s="10">
+        <v>4</v>
+      </c>
       <c r="G28" s="10"/>
       <c r="H28" s="10"/>
       <c r="I28" s="10"/>
@@ -4645,27 +4665,27 @@
       </c>
       <c r="M28" s="20">
         <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=3")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N28" s="20">
         <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=4")</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="O28" s="20">
         <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=5")</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="P28" s="20">
         <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=6")</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="Q28" s="20">
         <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=7")</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="R28" s="20">
         <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=8")</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="S28" s="20">
         <f>SUMIF(Table5[[#This Row],[A]:[E]],"&lt;=FILL THIS IN")</f>
@@ -4717,46 +4737,56 @@
       <c r="A29" s="9">
         <v>113</v>
       </c>
-      <c r="B29" s="10"/>
-      <c r="C29" s="10"/>
-      <c r="D29" s="10"/>
-      <c r="E29" s="10"/>
-      <c r="F29" s="10"/>
+      <c r="B29" s="10">
+        <v>1</v>
+      </c>
+      <c r="C29" s="10">
+        <v>5</v>
+      </c>
+      <c r="D29" s="10">
+        <v>2</v>
+      </c>
+      <c r="E29" s="10">
+        <v>3</v>
+      </c>
+      <c r="F29" s="10">
+        <v>5</v>
+      </c>
       <c r="G29" s="10"/>
       <c r="H29" s="10"/>
       <c r="I29" s="10"/>
       <c r="J29" s="11"/>
       <c r="K29" s="19">
         <f>COUNTIF(Table5[[#This Row],[A]:[E]], 1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L29" s="20">
         <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=2")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M29" s="20">
         <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=3")</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="N29" s="20">
         <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=4")</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="O29" s="20">
         <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=5")</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="P29" s="20">
         <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=6")</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="Q29" s="20">
         <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=7")</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="R29" s="20">
         <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=8")</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="S29" s="20">
         <f>SUMIF(Table5[[#This Row],[A]:[E]],"&lt;=FILL THIS IN")</f>
@@ -4808,46 +4838,56 @@
       <c r="A30" s="9">
         <v>114</v>
       </c>
-      <c r="B30" s="10"/>
-      <c r="C30" s="10"/>
-      <c r="D30" s="10"/>
-      <c r="E30" s="10"/>
-      <c r="F30" s="10"/>
+      <c r="B30" s="10">
+        <v>3</v>
+      </c>
+      <c r="C30" s="10">
+        <v>3</v>
+      </c>
+      <c r="D30" s="10">
+        <v>4</v>
+      </c>
+      <c r="E30" s="10">
+        <v>5</v>
+      </c>
+      <c r="F30" s="10">
+        <v>1</v>
+      </c>
       <c r="G30" s="10"/>
       <c r="H30" s="10"/>
       <c r="I30" s="10"/>
       <c r="J30" s="11"/>
       <c r="K30" s="19">
         <f>COUNTIF(Table5[[#This Row],[A]:[E]], 1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L30" s="20">
         <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=2")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M30" s="20">
         <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=3")</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="N30" s="20">
         <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=4")</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="O30" s="20">
         <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=5")</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="P30" s="20">
         <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=6")</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="Q30" s="20">
         <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=7")</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="R30" s="20">
         <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=8")</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="S30" s="20">
         <f>SUMIF(Table5[[#This Row],[A]:[E]],"&lt;=FILL THIS IN")</f>
@@ -4899,46 +4939,56 @@
       <c r="A31" s="9">
         <v>115</v>
       </c>
-      <c r="B31" s="10"/>
-      <c r="C31" s="10"/>
-      <c r="D31" s="10"/>
-      <c r="E31" s="10"/>
-      <c r="F31" s="10"/>
+      <c r="B31" s="10">
+        <v>2</v>
+      </c>
+      <c r="C31" s="10">
+        <v>1</v>
+      </c>
+      <c r="D31" s="10">
+        <v>1</v>
+      </c>
+      <c r="E31" s="10">
+        <v>2</v>
+      </c>
+      <c r="F31" s="10">
+        <v>2</v>
+      </c>
       <c r="G31" s="10"/>
       <c r="H31" s="10"/>
       <c r="I31" s="10"/>
       <c r="J31" s="11"/>
       <c r="K31" s="22">
         <f>COUNTIF(Table5[[#This Row],[A]:[E]], 1)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L31" s="23">
         <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=2")</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="M31" s="23">
         <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=3")</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="N31" s="23">
         <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=4")</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="O31" s="23">
         <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=5")</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="P31" s="23">
         <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=6")</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="Q31" s="23">
         <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=7")</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="R31" s="23">
         <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=8")</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="S31" s="23">
         <f>SUMIF(Table5[[#This Row],[A]:[E]],"&lt;=FILL THIS IN")</f>
@@ -4990,46 +5040,56 @@
       <c r="A32" s="9">
         <v>116</v>
       </c>
-      <c r="B32" s="10"/>
-      <c r="C32" s="10"/>
-      <c r="D32" s="10"/>
-      <c r="E32" s="10"/>
-      <c r="F32" s="10"/>
+      <c r="B32" s="10">
+        <v>5</v>
+      </c>
+      <c r="C32" s="10">
+        <v>4</v>
+      </c>
+      <c r="D32" s="10">
+        <v>6</v>
+      </c>
+      <c r="E32" s="10">
+        <v>1</v>
+      </c>
+      <c r="F32" s="10">
+        <v>3</v>
+      </c>
       <c r="G32" s="10"/>
       <c r="H32" s="10"/>
       <c r="I32" s="10"/>
       <c r="J32" s="11"/>
       <c r="K32" s="19">
         <f>COUNTIF(Table5[[#This Row],[A]:[E]], 1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L32" s="20">
         <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=2")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M32" s="20">
         <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=3")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N32" s="20">
         <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=4")</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="O32" s="20">
         <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=5")</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="P32" s="20">
         <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=6")</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="Q32" s="20">
         <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=7")</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="R32" s="20">
         <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=8")</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="S32" s="20">
         <f>SUMIF(Table5[[#This Row],[A]:[E]],"&lt;=FILL THIS IN")</f>
@@ -5081,11 +5141,21 @@
       <c r="A33" s="12">
         <v>117</v>
       </c>
-      <c r="B33" s="13"/>
-      <c r="C33" s="13"/>
-      <c r="D33" s="13"/>
-      <c r="E33" s="13"/>
-      <c r="F33" s="13"/>
+      <c r="B33" s="13">
+        <v>6</v>
+      </c>
+      <c r="C33" s="13">
+        <v>2</v>
+      </c>
+      <c r="D33" s="13">
+        <v>5</v>
+      </c>
+      <c r="E33" s="13">
+        <v>4</v>
+      </c>
+      <c r="F33" s="13">
+        <v>6</v>
+      </c>
       <c r="G33" s="13"/>
       <c r="H33" s="13"/>
       <c r="I33" s="13"/>
@@ -5096,31 +5166,31 @@
       </c>
       <c r="L33" s="26">
         <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=2")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M33" s="26">
         <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=3")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N33" s="26">
         <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=4")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O33" s="26">
         <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=5")</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="P33" s="26">
         <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=6")</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="Q33" s="26">
         <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=7")</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="R33" s="26">
         <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=8")</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="S33" s="26">
         <f>SUMIF(Table5[[#This Row],[A]:[E]],"&lt;=FILL THIS IN")</f>

</xml_diff>

<commit_message>
Trying to remove the tied couples and handle the fact that they need to be saved differently
</commit_message>
<xml_diff>
--- a/Dance Competition Sheet.xlsx
+++ b/Dance Competition Sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adammcpherson/Documents/DM1/TA/DanceCompetition/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F834A67A-32F4-C34A-BFB7-B81F3CEB908C}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9913823E-83B6-524A-A48C-AB73F46C5893}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{D9D28937-1BC5-C94D-91B6-1BFC68270A7E}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{D9D28937-1BC5-C94D-91B6-1BFC68270A7E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="45">
   <si>
     <t xml:space="preserve">No. </t>
   </si>
@@ -155,6 +155,12 @@
   <si>
     <t>EX: 116</t>
   </si>
+  <si>
+    <t>Tied 2</t>
+  </si>
+  <si>
+    <t>Tied 4</t>
+  </si>
 </sst>
 </file>
 
@@ -862,7 +868,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -885,9 +891,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -929,24 +933,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="40" xfId="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="49" xfId="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="45" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -954,21 +940,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -995,6 +966,43 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -1002,6 +1010,111 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="87">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Helvetica"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thick">
+          <color auto="1"/>
+        </left>
+      </border>
+    </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thick">
@@ -3425,7 +3538,7 @@
         </patternFill>
       </fill>
       <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
+        <left style="thick">
           <color auto="1"/>
         </left>
         <right style="thin">
@@ -3446,112 +3559,7 @@
       </border>
     </dxf>
     <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thick">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
       <border diagonalUp="0" diagonalDown="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Helvetica"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thick">
-          <color auto="1"/>
-        </left>
-      </border>
     </dxf>
     <dxf>
       <border outline="0">
@@ -3830,7 +3838,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{A958EBC6-E5F9-FA41-8059-1514ABF7AAB6}" name="Table5" displayName="Table5" ref="A26:V33" totalsRowShown="0" headerRowDxfId="86" headerRowBorderDxfId="85" tableBorderDxfId="84" headerRowCellStyle="Check Cell">
   <autoFilter ref="A26:V33" xr:uid="{18BC5C1E-6C7F-C542-9C1F-F30AB8500471}"/>
   <tableColumns count="22">
-    <tableColumn id="1" xr3:uid="{57D02D44-66F8-094D-A76F-6C1117FE30CE}" name="No. " dataDxfId="83"/>
+    <tableColumn id="1" xr3:uid="{57D02D44-66F8-094D-A76F-6C1117FE30CE}" name="No. " dataDxfId="2"/>
     <tableColumn id="2" xr3:uid="{8573DB78-D3F6-9B45-B90F-232F0946DBFA}" name="A"/>
     <tableColumn id="3" xr3:uid="{C4C572C3-2C00-1645-A12C-65D22A358FB8}" name="B"/>
     <tableColumn id="4" xr3:uid="{4D5F7649-4742-3842-9806-2161D13B3144}" name="C"/>
@@ -3839,49 +3847,49 @@
     <tableColumn id="7" xr3:uid="{AA514D78-B7B6-1743-BAFD-15B51C407E29}" name="F"/>
     <tableColumn id="8" xr3:uid="{EF3B4FBB-0C8D-554E-8B02-F92BC8B72E85}" name="G"/>
     <tableColumn id="9" xr3:uid="{5552FB60-D882-4A47-8164-EC8DDA1384E1}" name="H"/>
-    <tableColumn id="10" xr3:uid="{1B8CC32E-A213-3249-8C8C-A3C3B5B750A1}" name="J" dataDxfId="82"/>
-    <tableColumn id="12" xr3:uid="{156ABA9E-C91A-A344-992E-53D9C21B358A}" name="1" dataDxfId="81">
+    <tableColumn id="10" xr3:uid="{1B8CC32E-A213-3249-8C8C-A3C3B5B750A1}" name="J" dataDxfId="83"/>
+    <tableColumn id="12" xr3:uid="{156ABA9E-C91A-A344-992E-53D9C21B358A}" name="1" dataDxfId="82">
       <calculatedColumnFormula>COUNTIF(Table5[[#This Row],[A]:[E]], 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{45849B2A-AAF6-7246-890F-BDD97062F6E5}" name="1-2" dataDxfId="80">
+    <tableColumn id="13" xr3:uid="{45849B2A-AAF6-7246-890F-BDD97062F6E5}" name="1-2" dataDxfId="81">
       <calculatedColumnFormula>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=2")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{73E793AD-5B0C-784F-9C8E-AE19B507B943}" name="1-3" dataDxfId="79">
+    <tableColumn id="14" xr3:uid="{73E793AD-5B0C-784F-9C8E-AE19B507B943}" name="1-3" dataDxfId="80">
       <calculatedColumnFormula>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=3")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{B45B4FCD-82BA-6A4B-851C-7351CF347767}" name="1-4" dataDxfId="78">
+    <tableColumn id="15" xr3:uid="{B45B4FCD-82BA-6A4B-851C-7351CF347767}" name="1-4" dataDxfId="79">
       <calculatedColumnFormula>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=4")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{18463E75-07E6-BB4A-8411-986326C0EA8E}" name="1-5" dataDxfId="77">
+    <tableColumn id="16" xr3:uid="{18463E75-07E6-BB4A-8411-986326C0EA8E}" name="1-5" dataDxfId="78">
       <calculatedColumnFormula>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=5")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{39B70CC5-6485-4140-920B-04E1BC357026}" name="1-6" dataDxfId="76">
+    <tableColumn id="17" xr3:uid="{39B70CC5-6485-4140-920B-04E1BC357026}" name="1-6" dataDxfId="77">
       <calculatedColumnFormula>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=6")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{7CC4A663-FA21-D743-B0CC-EDC891AD5332}" name="1-7" dataDxfId="75">
+    <tableColumn id="18" xr3:uid="{7CC4A663-FA21-D743-B0CC-EDC891AD5332}" name="1-7" dataDxfId="76">
       <calculatedColumnFormula>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=7")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{20E3E48C-7599-8748-A2BC-44EBFF5C0FC6}" name="1-8" dataDxfId="74">
+    <tableColumn id="19" xr3:uid="{20E3E48C-7599-8748-A2BC-44EBFF5C0FC6}" name="1-8" dataDxfId="75">
       <calculatedColumnFormula>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=8")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="23" xr3:uid="{B364F798-7E28-924D-87E4-E35465876C7A}" name="Tie Break#1" dataDxfId="73">
-      <calculatedColumnFormula>SUMIF(Table5[[#This Row],[A]:[E]],"&lt;=FILL THIS IN")</calculatedColumnFormula>
+    <tableColumn id="23" xr3:uid="{B364F798-7E28-924D-87E4-E35465876C7A}" name="Tie Break#1" dataDxfId="1">
+      <calculatedColumnFormula>SUMIF(Table5[[#This Row],[A]:[E]],"&lt;=2")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="24" xr3:uid="{78237D1A-EB91-9747-A330-01A46FBB2742}" name="Tie Break#2" dataDxfId="72">
-      <calculatedColumnFormula>SUMIF(Table5[[#This Row],[A]:[E]],"&lt;=FILL THIS IN")</calculatedColumnFormula>
+    <tableColumn id="24" xr3:uid="{78237D1A-EB91-9747-A330-01A46FBB2742}" name="Tie Break#2" dataDxfId="0">
+      <calculatedColumnFormula>SUMIF(Table5[[#This Row],[A]:[E]],"&lt;=3")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="25" xr3:uid="{69161E1A-D6D1-5C41-97A2-1B54F51DDF5F}" name="Tie Break#3" dataDxfId="71"/>
-    <tableColumn id="20" xr3:uid="{8D4BC117-F86E-FA48-AF1D-B5D11B9C7CBA}" name="Result" dataDxfId="70"/>
+    <tableColumn id="25" xr3:uid="{69161E1A-D6D1-5C41-97A2-1B54F51DDF5F}" name="Tie Break#3" dataDxfId="74"/>
+    <tableColumn id="20" xr3:uid="{8D4BC117-F86E-FA48-AF1D-B5D11B9C7CBA}" name="Result" dataDxfId="73"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{E50215A1-CE1B-F24B-A3A4-F70D1E7C8C28}" name="Table6" displayName="Table6" ref="A35:J42" totalsRowShown="0" headerRowDxfId="69" headerRowBorderDxfId="68" tableBorderDxfId="67" headerRowCellStyle="Check Cell">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{E50215A1-CE1B-F24B-A3A4-F70D1E7C8C28}" name="Table6" displayName="Table6" ref="A35:J42" totalsRowShown="0" headerRowDxfId="72" headerRowBorderDxfId="71" tableBorderDxfId="70" headerRowCellStyle="Check Cell">
   <autoFilter ref="A35:J42" xr:uid="{822117C4-C240-004D-9F32-86F10EF15DB6}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{CE4A6080-428A-9F4C-B252-8FA7A878FBA7}" name="No. " dataDxfId="66">
+    <tableColumn id="1" xr3:uid="{CE4A6080-428A-9F4C-B252-8FA7A878FBA7}" name="No. " dataDxfId="69">
       <calculatedColumnFormula>A27</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="2" xr3:uid="{91B188C1-5953-B947-9C2F-3BC1268D9E07}" name="A"/>
@@ -3899,10 +3907,10 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{CD4A6E3E-1AF9-4141-A681-18758A14C3C1}" name="Table7" displayName="Table7" ref="A44:J51" totalsRowShown="0" headerRowDxfId="65" headerRowBorderDxfId="64" tableBorderDxfId="63" headerRowCellStyle="Check Cell">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{CD4A6E3E-1AF9-4141-A681-18758A14C3C1}" name="Table7" displayName="Table7" ref="A44:J51" totalsRowShown="0" headerRowDxfId="68" headerRowBorderDxfId="67" tableBorderDxfId="66" headerRowCellStyle="Check Cell">
   <autoFilter ref="A44:J51" xr:uid="{FA9CCF3B-D2B7-8745-911A-41DE0BA2D56E}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{BF3E417C-E88A-B249-B957-C4374548B35A}" name="No. " dataDxfId="62">
+    <tableColumn id="1" xr3:uid="{BF3E417C-E88A-B249-B957-C4374548B35A}" name="No. " dataDxfId="65">
       <calculatedColumnFormula>A27</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="2" xr3:uid="{560C67EF-0E22-1D49-915D-041AF7EA89CB}" name="A"/>
@@ -3920,10 +3928,10 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{5C91623F-864E-C141-8F75-3BD6D8A745C4}" name="Table8" displayName="Table8" ref="A53:J60" totalsRowShown="0" headerRowDxfId="61" headerRowBorderDxfId="60" tableBorderDxfId="59" headerRowCellStyle="Check Cell">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{5C91623F-864E-C141-8F75-3BD6D8A745C4}" name="Table8" displayName="Table8" ref="A53:J60" totalsRowShown="0" headerRowDxfId="64" headerRowBorderDxfId="63" tableBorderDxfId="62" headerRowCellStyle="Check Cell">
   <autoFilter ref="A53:J60" xr:uid="{27316687-9F4B-9744-8676-B09D0E875569}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{B3DBCB62-FB2D-C645-9515-B356F5EAEF29}" name="No. " dataDxfId="58">
+    <tableColumn id="1" xr3:uid="{B3DBCB62-FB2D-C645-9515-B356F5EAEF29}" name="No. " dataDxfId="61">
       <calculatedColumnFormula>A27</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="2" xr3:uid="{2D0B4B6B-9866-B847-A7FC-C3BCC560EF8B}" name="A"/>
@@ -3941,141 +3949,141 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{30D2BDB7-2519-4E4F-877F-8D6AEE2DF935}" name="Table4" displayName="Table4" ref="K35:V42" totalsRowShown="0" headerRowDxfId="57" dataDxfId="56" tableBorderDxfId="55" headerRowCellStyle="Check Cell">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{30D2BDB7-2519-4E4F-877F-8D6AEE2DF935}" name="Table4" displayName="Table4" ref="K35:V42" totalsRowShown="0" headerRowDxfId="60" dataDxfId="59" tableBorderDxfId="58" headerRowCellStyle="Check Cell">
   <autoFilter ref="K35:V42" xr:uid="{26E39BDB-BA98-CD48-AFFD-A777B858DF4A}"/>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{D0975B44-86FE-6E4C-BA72-D2D7B49F5328}" name="1" dataDxfId="54">
+    <tableColumn id="1" xr3:uid="{D0975B44-86FE-6E4C-BA72-D2D7B49F5328}" name="1" dataDxfId="57">
       <calculatedColumnFormula>COUNTIF(Table6[[#This Row],[A]:[E]], 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{D0228C96-2F36-9B4A-B834-63688503BC38}" name="1-2" dataDxfId="53">
+    <tableColumn id="2" xr3:uid="{D0228C96-2F36-9B4A-B834-63688503BC38}" name="1-2" dataDxfId="56">
       <calculatedColumnFormula>COUNTIF(Table6[[#This Row],[A]:[E]],"&lt;=2")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{3E58F420-F6AD-944D-ABD9-7C64E05E357A}" name="1-3" dataDxfId="52">
+    <tableColumn id="3" xr3:uid="{3E58F420-F6AD-944D-ABD9-7C64E05E357A}" name="1-3" dataDxfId="55">
       <calculatedColumnFormula>COUNTIF(Table6[[#This Row],[A]:[E]],"&lt;=3")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{AF60E446-AE28-BE4B-82CD-80739F1F319C}" name="1-4" dataDxfId="51">
+    <tableColumn id="4" xr3:uid="{AF60E446-AE28-BE4B-82CD-80739F1F319C}" name="1-4" dataDxfId="54">
       <calculatedColumnFormula>COUNTIF(Table6[[#This Row],[A]:[E]],"&lt;=4")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{C5257B58-87BF-5649-903C-9A0949A2DBB9}" name="1-5" dataDxfId="50">
+    <tableColumn id="5" xr3:uid="{C5257B58-87BF-5649-903C-9A0949A2DBB9}" name="1-5" dataDxfId="53">
       <calculatedColumnFormula>COUNTIF(Table6[[#This Row],[A]:[E]],"&lt;=5")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{BA2605CD-9918-1741-BAA6-E634E1B73E71}" name="1-6" dataDxfId="49">
+    <tableColumn id="6" xr3:uid="{BA2605CD-9918-1741-BAA6-E634E1B73E71}" name="1-6" dataDxfId="52">
       <calculatedColumnFormula>COUNTIF(Table6[[#This Row],[A]:[E]],"&lt;=6")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{0AC0B5C0-0436-BA4B-AC13-9922E8EDBA63}" name="1-7" dataDxfId="48">
+    <tableColumn id="7" xr3:uid="{0AC0B5C0-0436-BA4B-AC13-9922E8EDBA63}" name="1-7" dataDxfId="51">
       <calculatedColumnFormula>COUNTIF(Table6[[#This Row],[A]:[E]],"&lt;=7")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{D0C7A017-2835-F840-87DC-7E16E1B47202}" name="1-8" dataDxfId="47">
+    <tableColumn id="8" xr3:uid="{D0C7A017-2835-F840-87DC-7E16E1B47202}" name="1-8" dataDxfId="50">
       <calculatedColumnFormula>COUNTIF(Table6[[#This Row],[A]:[E]],"&lt;=8")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{64D463FA-C7F3-B645-8251-0EAA7892BC33}" name="Tie Break#1" dataDxfId="46">
+    <tableColumn id="9" xr3:uid="{64D463FA-C7F3-B645-8251-0EAA7892BC33}" name="Tie Break#1" dataDxfId="49">
       <calculatedColumnFormula>SUMIF(Table6[[#This Row],[A]:[E]],"&lt;=FILL THIS IN")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{1DB664C4-D158-D94D-96E8-041633D0EF28}" name="Tie Break#2" dataDxfId="45"/>
-    <tableColumn id="11" xr3:uid="{D3C8A54C-AAEF-BF43-90B4-635FAEC73806}" name="Tie Break#3" dataDxfId="44"/>
-    <tableColumn id="12" xr3:uid="{8DBD5070-CA95-7140-B44E-C8FBCDB0583A}" name="Result" dataDxfId="43"/>
+    <tableColumn id="10" xr3:uid="{1DB664C4-D158-D94D-96E8-041633D0EF28}" name="Tie Break#2" dataDxfId="48"/>
+    <tableColumn id="11" xr3:uid="{D3C8A54C-AAEF-BF43-90B4-635FAEC73806}" name="Tie Break#3" dataDxfId="47"/>
+    <tableColumn id="12" xr3:uid="{8DBD5070-CA95-7140-B44E-C8FBCDB0583A}" name="Result" dataDxfId="46"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{673EDB5E-9FFE-DE47-A1A6-BEB6E1ED35C5}" name="Table9" displayName="Table9" ref="K44:V51" totalsRowShown="0" headerRowDxfId="42" dataDxfId="41" tableBorderDxfId="40" headerRowCellStyle="Check Cell">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{673EDB5E-9FFE-DE47-A1A6-BEB6E1ED35C5}" name="Table9" displayName="Table9" ref="K44:V51" totalsRowShown="0" headerRowDxfId="45" dataDxfId="44" tableBorderDxfId="43" headerRowCellStyle="Check Cell">
   <autoFilter ref="K44:V51" xr:uid="{B523455A-032F-1347-A148-D603C31BEF08}"/>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{1C7030AE-6933-6F44-9068-516479D47978}" name="1" dataDxfId="39">
+    <tableColumn id="1" xr3:uid="{1C7030AE-6933-6F44-9068-516479D47978}" name="1" dataDxfId="42">
       <calculatedColumnFormula>COUNTIF(Table7[[#This Row],[A]:[E]], 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{1D58BD74-3AF2-3D46-AD68-8BFA8E4249F6}" name="1-2" dataDxfId="38">
+    <tableColumn id="2" xr3:uid="{1D58BD74-3AF2-3D46-AD68-8BFA8E4249F6}" name="1-2" dataDxfId="41">
       <calculatedColumnFormula>COUNTIF(Table7[[#This Row],[A]:[E]],"&lt;=2")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{95A66C98-7203-8E45-9B6B-0D73457D792C}" name="1-3" dataDxfId="37">
+    <tableColumn id="3" xr3:uid="{95A66C98-7203-8E45-9B6B-0D73457D792C}" name="1-3" dataDxfId="40">
       <calculatedColumnFormula>COUNTIF(Table7[[#This Row],[A]:[E]],"&lt;=3")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{338A0E85-9F7B-6549-A25B-45479E4C62CD}" name="1-4" dataDxfId="36">
+    <tableColumn id="4" xr3:uid="{338A0E85-9F7B-6549-A25B-45479E4C62CD}" name="1-4" dataDxfId="39">
       <calculatedColumnFormula>COUNTIF(Table7[[#This Row],[A]:[E]],"&lt;=4")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{F844FD21-C43D-5A4A-BE27-9789848BE13A}" name="1-5" dataDxfId="35">
+    <tableColumn id="5" xr3:uid="{F844FD21-C43D-5A4A-BE27-9789848BE13A}" name="1-5" dataDxfId="38">
       <calculatedColumnFormula>COUNTIF(Table7[[#This Row],[A]:[E]],"&lt;=5")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{20BD4D82-0CD2-5D42-B65E-63BCAEFC6C53}" name="1-6" dataDxfId="34">
+    <tableColumn id="6" xr3:uid="{20BD4D82-0CD2-5D42-B65E-63BCAEFC6C53}" name="1-6" dataDxfId="37">
       <calculatedColumnFormula>COUNTIF(Table7[[#This Row],[A]:[E]],"&lt;=6")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{FF0ABED5-0187-664A-A47E-FAF0FBF8EEAA}" name="1-7" dataDxfId="33">
+    <tableColumn id="7" xr3:uid="{FF0ABED5-0187-664A-A47E-FAF0FBF8EEAA}" name="1-7" dataDxfId="36">
       <calculatedColumnFormula>COUNTIF(Table7[[#This Row],[A]:[E]],"&lt;=7")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{E17E2343-53C8-4444-A35A-CF801ABDBF73}" name="1-8" dataDxfId="32">
+    <tableColumn id="8" xr3:uid="{E17E2343-53C8-4444-A35A-CF801ABDBF73}" name="1-8" dataDxfId="35">
       <calculatedColumnFormula>COUNTIF(Table7[[#This Row],[A]:[E]],"&lt;=8")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{6AB229FE-797D-C84D-9437-074DCF356DB8}" name="Tie Break#1" dataDxfId="31">
+    <tableColumn id="9" xr3:uid="{6AB229FE-797D-C84D-9437-074DCF356DB8}" name="Tie Break#1" dataDxfId="34">
       <calculatedColumnFormula>SUMIF(Table7[[#This Row],[A]:[E]],"&lt;=FILL THIS IN")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{C66E0318-0575-114C-BA31-61617D8296AC}" name="Tie Break#2" dataDxfId="30"/>
-    <tableColumn id="11" xr3:uid="{935B59A3-BD5D-2041-BB60-999DD3FDA879}" name="Tie Break#3" dataDxfId="29"/>
-    <tableColumn id="12" xr3:uid="{094A5396-AC72-CD46-93EE-0738007C3426}" name="Result" dataDxfId="28"/>
+    <tableColumn id="10" xr3:uid="{C66E0318-0575-114C-BA31-61617D8296AC}" name="Tie Break#2" dataDxfId="33"/>
+    <tableColumn id="11" xr3:uid="{935B59A3-BD5D-2041-BB60-999DD3FDA879}" name="Tie Break#3" dataDxfId="32"/>
+    <tableColumn id="12" xr3:uid="{094A5396-AC72-CD46-93EE-0738007C3426}" name="Result" dataDxfId="31"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{4850EA14-CB5F-4943-94EF-83331955AB6A}" name="Table10" displayName="Table10" ref="K53:V60" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26" tableBorderDxfId="25" headerRowCellStyle="Check Cell">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{4850EA14-CB5F-4943-94EF-83331955AB6A}" name="Table10" displayName="Table10" ref="K53:V60" totalsRowShown="0" headerRowDxfId="30" dataDxfId="29" tableBorderDxfId="28" headerRowCellStyle="Check Cell">
   <autoFilter ref="K53:V60" xr:uid="{6927E80A-15A3-BB47-9D79-AA4675019CC9}"/>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{33905209-BFFE-9540-AC95-91CE599F15B3}" name="1" dataDxfId="24">
+    <tableColumn id="1" xr3:uid="{33905209-BFFE-9540-AC95-91CE599F15B3}" name="1" dataDxfId="27">
       <calculatedColumnFormula>COUNTIF(Table8[[#This Row],[A]:[E]], 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{0FE07D2F-3F07-2741-A1A8-669F800872B6}" name="1-2" dataDxfId="23">
+    <tableColumn id="2" xr3:uid="{0FE07D2F-3F07-2741-A1A8-669F800872B6}" name="1-2" dataDxfId="26">
       <calculatedColumnFormula>COUNTIF(Table8[[#This Row],[A]:[E]],"&lt;=2")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{20BF183A-E7BA-4B4A-97D4-5E94EB00D03F}" name="1-3" dataDxfId="22">
+    <tableColumn id="3" xr3:uid="{20BF183A-E7BA-4B4A-97D4-5E94EB00D03F}" name="1-3" dataDxfId="25">
       <calculatedColumnFormula>COUNTIF(Table8[[#This Row],[A]:[E]],"&lt;=3")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{85379A8A-3CC7-4544-BEF4-A1AE3F76402F}" name="1-4" dataDxfId="21">
+    <tableColumn id="4" xr3:uid="{85379A8A-3CC7-4544-BEF4-A1AE3F76402F}" name="1-4" dataDxfId="24">
       <calculatedColumnFormula>COUNTIF(Table8[[#This Row],[A]:[E]],"&lt;=4")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{C82212E8-8D29-514E-8A29-0DC18134A709}" name="1-5" dataDxfId="20">
+    <tableColumn id="5" xr3:uid="{C82212E8-8D29-514E-8A29-0DC18134A709}" name="1-5" dataDxfId="23">
       <calculatedColumnFormula>COUNTIF(Table8[[#This Row],[A]:[E]],"&lt;=5")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{A6182525-C2FF-B549-9202-2326F1ADCD83}" name="1-6" dataDxfId="19">
+    <tableColumn id="6" xr3:uid="{A6182525-C2FF-B549-9202-2326F1ADCD83}" name="1-6" dataDxfId="22">
       <calculatedColumnFormula>COUNTIF(Table8[[#This Row],[A]:[E]],"&lt;=6")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{651CB0C2-0330-304E-A333-ED2458AAC703}" name="1-7" dataDxfId="18">
+    <tableColumn id="7" xr3:uid="{651CB0C2-0330-304E-A333-ED2458AAC703}" name="1-7" dataDxfId="21">
       <calculatedColumnFormula>COUNTIF(Table8[[#This Row],[A]:[E]],"&lt;=7")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{C19C5A08-DFB6-E044-9F49-FF57456220AF}" name="1-8" dataDxfId="17">
+    <tableColumn id="8" xr3:uid="{C19C5A08-DFB6-E044-9F49-FF57456220AF}" name="1-8" dataDxfId="20">
       <calculatedColumnFormula>COUNTIF(Table8[[#This Row],[A]:[E]],"&lt;=8")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{8C93F823-C7ED-FC4A-BDBF-905649725DB1}" name="RuleBreak#1" dataDxfId="16">
+    <tableColumn id="9" xr3:uid="{8C93F823-C7ED-FC4A-BDBF-905649725DB1}" name="RuleBreak#1" dataDxfId="19">
       <calculatedColumnFormula>SUMIF(Table8[[#This Row],[A]:[E]],"&lt;=FILL THIS IN")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{1793E772-2C95-5143-A99B-15789DFB1FC6}" name="RuleBreak#2" dataDxfId="15"/>
-    <tableColumn id="11" xr3:uid="{0BD975F0-58C0-6A4D-8C71-C1E8BBA50A2E}" name="RuleBreak#3" dataDxfId="14"/>
-    <tableColumn id="12" xr3:uid="{C137F097-C242-CD44-A736-4844E26F42AA}" name="Result" dataDxfId="13"/>
+    <tableColumn id="10" xr3:uid="{1793E772-2C95-5143-A99B-15789DFB1FC6}" name="RuleBreak#2" dataDxfId="18"/>
+    <tableColumn id="11" xr3:uid="{0BD975F0-58C0-6A4D-8C71-C1E8BBA50A2E}" name="RuleBreak#3" dataDxfId="17"/>
+    <tableColumn id="12" xr3:uid="{C137F097-C242-CD44-A736-4844E26F42AA}" name="Result" dataDxfId="16"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{B5916B0A-D6C7-1D4F-A16F-4E69C679226F}" name="Table11" displayName="Table11" ref="X26:AF34" totalsRowShown="0" headerRowDxfId="12" headerRowBorderDxfId="11" tableBorderDxfId="10" totalsRowBorderDxfId="9" headerRowCellStyle="Check Cell">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{B5916B0A-D6C7-1D4F-A16F-4E69C679226F}" name="Table11" displayName="Table11" ref="X26:AF34" totalsRowShown="0" headerRowDxfId="15" headerRowBorderDxfId="14" tableBorderDxfId="13" totalsRowBorderDxfId="12" headerRowCellStyle="Check Cell">
   <autoFilter ref="X26:AF34" xr:uid="{72A9FCD0-51BB-9141-A84C-18D48B93E5C4}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{B81CE214-AED0-4342-9DAB-07D70839F3CE}" name="No. " dataDxfId="8">
+    <tableColumn id="1" xr3:uid="{B81CE214-AED0-4342-9DAB-07D70839F3CE}" name="No. " dataDxfId="11">
       <calculatedColumnFormula>Table5[[#This Row],[No. ]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{E70AB7D8-9F24-CF45-A411-9F91A822B337}" name="C" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{A6C623A5-8425-C540-A1C4-F547B709B159}" name="R" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{B42DA36A-B7F4-AA45-8CDB-07B3B3476183}" name="S" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{B25C0C43-8E3F-404C-B69D-E0D1B6E6D6FB}" name="M" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{CA7D191A-55C4-C54E-98F2-7B07116BA8AB}" name="Tie Break#1" dataDxfId="3">
+    <tableColumn id="2" xr3:uid="{E70AB7D8-9F24-CF45-A411-9F91A822B337}" name="C" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{A6C623A5-8425-C540-A1C4-F547B709B159}" name="R" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{B42DA36A-B7F4-AA45-8CDB-07B3B3476183}" name="S" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{B25C0C43-8E3F-404C-B69D-E0D1B6E6D6FB}" name="M" dataDxfId="7"/>
+    <tableColumn id="6" xr3:uid="{CA7D191A-55C4-C54E-98F2-7B07116BA8AB}" name="Tie Break#1" dataDxfId="6">
       <calculatedColumnFormula>COUNTIF(Table11[[#This Row],[C]:[M]],"&lt;=FILL THIS IN")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{38C06049-7E80-E847-8DF7-D8B0260D3112}" name="Tie Break SUM #2" dataDxfId="2">
+    <tableColumn id="7" xr3:uid="{38C06049-7E80-E847-8DF7-D8B0260D3112}" name="Tie Break SUM #2" dataDxfId="5">
       <calculatedColumnFormula>COUNTIF(Table11[[#This Row],[C]:[M]],"&lt;=FILL THIS IN")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{E6450403-7FEC-1244-A0C6-C37D9D2A68B4}" name="Total" dataDxfId="1"/>
-    <tableColumn id="9" xr3:uid="{FACF3E14-FC2B-4B45-8CB3-D87FB5C2B678}" name="Result" dataDxfId="0"/>
+    <tableColumn id="8" xr3:uid="{E6450403-7FEC-1244-A0C6-C37D9D2A68B4}" name="Total" dataDxfId="4"/>
+    <tableColumn id="9" xr3:uid="{FACF3E14-FC2B-4B45-8CB3-D87FB5C2B678}" name="Result" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4380,8 +4388,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{728F71C9-42E1-6448-AE41-E1190B29DDE7}">
   <dimension ref="A2:AF61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="125" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="125" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="N1" activePane="topRight" state="frozen"/>
+      <selection activeCell="A16" sqref="A16"/>
+      <selection pane="topRight" activeCell="S28" sqref="S28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4396,43 +4406,43 @@
     </row>
     <row r="24" spans="1:32" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="25" spans="1:32" ht="20" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="83" t="s">
+      <c r="A25" s="70" t="s">
         <v>31</v>
       </c>
-      <c r="B25" s="86"/>
-      <c r="C25" s="86"/>
-      <c r="D25" s="86"/>
-      <c r="E25" s="86"/>
-      <c r="F25" s="86"/>
-      <c r="G25" s="86"/>
-      <c r="H25" s="86"/>
-      <c r="I25" s="86"/>
-      <c r="J25" s="87"/>
-      <c r="K25" s="72" t="s">
+      <c r="B25" s="73"/>
+      <c r="C25" s="73"/>
+      <c r="D25" s="73"/>
+      <c r="E25" s="73"/>
+      <c r="F25" s="73"/>
+      <c r="G25" s="73"/>
+      <c r="H25" s="73"/>
+      <c r="I25" s="73"/>
+      <c r="J25" s="74"/>
+      <c r="K25" s="64" t="s">
         <v>18</v>
       </c>
-      <c r="L25" s="73"/>
-      <c r="M25" s="73"/>
-      <c r="N25" s="73"/>
-      <c r="O25" s="73"/>
-      <c r="P25" s="73"/>
-      <c r="Q25" s="73"/>
-      <c r="R25" s="73"/>
-      <c r="S25" s="73"/>
-      <c r="T25" s="73"/>
-      <c r="U25" s="73"/>
-      <c r="V25" s="74"/>
-      <c r="X25" s="80" t="s">
+      <c r="L25" s="65"/>
+      <c r="M25" s="65"/>
+      <c r="N25" s="65"/>
+      <c r="O25" s="65"/>
+      <c r="P25" s="65"/>
+      <c r="Q25" s="65"/>
+      <c r="R25" s="65"/>
+      <c r="S25" s="65"/>
+      <c r="T25" s="65"/>
+      <c r="U25" s="65"/>
+      <c r="V25" s="66"/>
+      <c r="X25" s="67" t="s">
         <v>20</v>
       </c>
-      <c r="Y25" s="81"/>
-      <c r="Z25" s="81"/>
-      <c r="AA25" s="81"/>
-      <c r="AB25" s="81"/>
-      <c r="AC25" s="81"/>
-      <c r="AD25" s="81"/>
-      <c r="AE25" s="81"/>
-      <c r="AF25" s="82"/>
+      <c r="Y25" s="68"/>
+      <c r="Z25" s="68"/>
+      <c r="AA25" s="68"/>
+      <c r="AB25" s="68"/>
+      <c r="AC25" s="68"/>
+      <c r="AD25" s="68"/>
+      <c r="AE25" s="68"/>
+      <c r="AF25" s="69"/>
     </row>
     <row r="26" spans="1:32" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
@@ -4465,28 +4475,28 @@
       <c r="J26" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K26" s="44" t="s">
+      <c r="K26" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="L26" s="36" t="s">
+      <c r="L26" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="M26" s="36" t="s">
+      <c r="M26" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="N26" s="36" t="s">
+      <c r="N26" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="O26" s="36" t="s">
+      <c r="O26" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="P26" s="36" t="s">
+      <c r="P26" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="Q26" s="36" t="s">
+      <c r="Q26" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="R26" s="43" t="s">
+      <c r="R26" s="41" t="s">
         <v>17</v>
       </c>
       <c r="S26" s="17" t="s">
@@ -4498,40 +4508,40 @@
       <c r="U26" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="V26" s="45" t="s">
+      <c r="V26" s="43" t="s">
         <v>19</v>
       </c>
-      <c r="X26" s="62" t="s">
-        <v>0</v>
-      </c>
-      <c r="Y26" s="63" t="s">
+      <c r="X26" s="60" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y26" s="61" t="s">
         <v>4</v>
       </c>
-      <c r="Z26" s="63" t="s">
+      <c r="Z26" s="61" t="s">
         <v>21</v>
       </c>
-      <c r="AA26" s="63" t="s">
+      <c r="AA26" s="61" t="s">
         <v>22</v>
       </c>
-      <c r="AB26" s="63" t="s">
+      <c r="AB26" s="61" t="s">
         <v>23</v>
       </c>
-      <c r="AC26" s="64" t="s">
+      <c r="AC26" s="62" t="s">
         <v>37</v>
       </c>
-      <c r="AD26" s="64" t="s">
+      <c r="AD26" s="62" t="s">
         <v>40</v>
       </c>
-      <c r="AE26" s="53" t="s">
+      <c r="AE26" s="51" t="s">
         <v>25</v>
       </c>
-      <c r="AF26" s="53" t="s">
+      <c r="AF26" s="51" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="27" spans="1:32" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A27" s="5">
-        <v>111</v>
+        <v>21</v>
       </c>
       <c r="B27" s="6">
         <v>7</v>
@@ -4540,7 +4550,7 @@
         <v>7</v>
       </c>
       <c r="D27" s="7">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E27" s="7">
         <v>7</v>
@@ -4552,182 +4562,184 @@
       <c r="H27" s="7"/>
       <c r="I27" s="7"/>
       <c r="J27" s="8"/>
-      <c r="K27" s="56">
+      <c r="K27" s="19">
         <f>COUNTIF(Table5[[#This Row],[A]:[E]], 1)</f>
         <v>0</v>
       </c>
-      <c r="L27" s="57">
+      <c r="L27" s="20">
         <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=2")</f>
         <v>0</v>
       </c>
-      <c r="M27" s="57">
+      <c r="M27" s="20">
         <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=3")</f>
         <v>0</v>
       </c>
-      <c r="N27" s="57">
+      <c r="N27" s="20">
         <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=4")</f>
-        <v>0</v>
-      </c>
-      <c r="O27" s="57">
+        <v>1</v>
+      </c>
+      <c r="O27" s="20">
         <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=5")</f>
-        <v>0</v>
-      </c>
-      <c r="P27" s="57">
+        <v>1</v>
+      </c>
+      <c r="P27" s="20">
         <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=6")</f>
-        <v>0</v>
-      </c>
-      <c r="Q27" s="57">
+        <v>1</v>
+      </c>
+      <c r="Q27" s="20">
         <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=7")</f>
         <v>5</v>
       </c>
-      <c r="R27" s="57">
+      <c r="R27" s="20">
         <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=8")</f>
         <v>5</v>
       </c>
-      <c r="S27" s="57">
-        <f>SUMIF(Table5[[#This Row],[A]:[E]],"&lt;=FILL THIS IN")</f>
-        <v>0</v>
-      </c>
-      <c r="T27" s="57">
-        <f>SUMIF(Table5[[#This Row],[A]:[E]],"&lt;=FILL THIS IN")</f>
-        <v>0</v>
-      </c>
-      <c r="U27" s="58"/>
-      <c r="V27" s="59">
+      <c r="S27" s="20">
+        <f>SUMIF(Table5[[#This Row],[A]:[E]],"&lt;=2")</f>
+        <v>0</v>
+      </c>
+      <c r="T27" s="20">
+        <f>SUMIF(Table5[[#This Row],[A]:[E]],"&lt;=3")</f>
+        <v>0</v>
+      </c>
+      <c r="U27" s="31"/>
+      <c r="V27" s="21">
         <v>7</v>
       </c>
-      <c r="X27" s="48">
+      <c r="X27" s="46">
         <f>Table5[[#This Row],[No. ]]</f>
-        <v>111</v>
-      </c>
-      <c r="Y27" s="46">
+        <v>21</v>
+      </c>
+      <c r="Y27" s="44">
         <f>Table5[[#This Row],[Result]]</f>
         <v>7</v>
       </c>
-      <c r="Z27" s="47">
+      <c r="Z27" s="45">
         <f t="shared" ref="Z27:Z33" si="0">V36</f>
         <v>0</v>
       </c>
-      <c r="AA27" s="47">
+      <c r="AA27" s="45">
         <f t="shared" ref="AA27:AA33" si="1">V45</f>
         <v>0</v>
       </c>
-      <c r="AB27" s="47">
+      <c r="AB27" s="45">
         <f t="shared" ref="AB27:AB33" si="2">V54</f>
         <v>0</v>
       </c>
-      <c r="AC27" s="47">
+      <c r="AC27" s="45">
         <f>COUNTIF(Table11[[#This Row],[C]:[M]],"&lt;=FILL THIS IN")</f>
         <v>0</v>
       </c>
-      <c r="AD27" s="60">
+      <c r="AD27" s="58">
         <f>SUMIF(Table11[[#This Row],[C]:[M]],"&lt;=FILL THIS IN")</f>
         <v>0</v>
       </c>
-      <c r="AE27" s="61">
+      <c r="AE27" s="59">
         <f>SUM(Y27:AD27)</f>
         <v>7</v>
       </c>
-      <c r="AF27" s="54">
+      <c r="AF27" s="52">
         <v>7</v>
       </c>
     </row>
     <row r="28" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A28" s="9">
-        <v>112</v>
+        <v>22</v>
       </c>
       <c r="B28" s="10">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C28" s="10">
+        <v>1</v>
+      </c>
+      <c r="D28" s="10">
+        <v>1</v>
+      </c>
+      <c r="E28" s="10">
+        <v>2</v>
+      </c>
+      <c r="F28" s="10">
         <v>6</v>
-      </c>
-      <c r="D28" s="10">
-        <v>3</v>
-      </c>
-      <c r="E28" s="10">
-        <v>6</v>
-      </c>
-      <c r="F28" s="10">
-        <v>4</v>
       </c>
       <c r="G28" s="10"/>
       <c r="H28" s="10"/>
       <c r="I28" s="10"/>
       <c r="J28" s="11"/>
-      <c r="K28" s="19">
+      <c r="K28" s="54">
         <f>COUNTIF(Table5[[#This Row],[A]:[E]], 1)</f>
-        <v>0</v>
-      </c>
-      <c r="L28" s="20">
+        <v>3</v>
+      </c>
+      <c r="L28" s="55">
         <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=2")</f>
-        <v>0</v>
-      </c>
-      <c r="M28" s="20">
+        <v>4</v>
+      </c>
+      <c r="M28" s="55">
         <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=3")</f>
-        <v>1</v>
-      </c>
-      <c r="N28" s="20">
+        <v>4</v>
+      </c>
+      <c r="N28" s="55">
         <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=4")</f>
-        <v>3</v>
-      </c>
-      <c r="O28" s="20">
+        <v>4</v>
+      </c>
+      <c r="O28" s="55">
         <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=5")</f>
-        <v>3</v>
-      </c>
-      <c r="P28" s="20">
+        <v>4</v>
+      </c>
+      <c r="P28" s="55">
         <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=6")</f>
         <v>5</v>
       </c>
-      <c r="Q28" s="20">
+      <c r="Q28" s="55">
         <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=7")</f>
         <v>5</v>
       </c>
-      <c r="R28" s="20">
+      <c r="R28" s="55">
         <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=8")</f>
         <v>5</v>
       </c>
-      <c r="S28" s="20">
-        <f>SUMIF(Table5[[#This Row],[A]:[E]],"&lt;=FILL THIS IN")</f>
-        <v>0</v>
-      </c>
-      <c r="T28" s="20">
-        <f>SUMIF(Table5[[#This Row],[A]:[E]],"&lt;=FILL THIS IN")</f>
-        <v>0</v>
-      </c>
-      <c r="U28" s="33"/>
-      <c r="V28" s="21"/>
-      <c r="X28" s="49">
+      <c r="S28" s="55">
+        <f>SUMIF(Table5[[#This Row],[A]:[E]],"&lt;=2")</f>
+        <v>5</v>
+      </c>
+      <c r="T28" s="55">
+        <f>SUMIF(Table5[[#This Row],[A]:[E]],"&lt;=3")</f>
+        <v>5</v>
+      </c>
+      <c r="U28" s="56"/>
+      <c r="V28" s="57">
+        <v>1</v>
+      </c>
+      <c r="X28" s="47">
         <f>Table5[[#This Row],[No. ]]</f>
-        <v>112</v>
-      </c>
-      <c r="Y28" s="46">
+        <v>22</v>
+      </c>
+      <c r="Y28" s="44">
         <f>Table5[[#This Row],[Result]]</f>
-        <v>0</v>
-      </c>
-      <c r="Z28" s="47">
+        <v>1</v>
+      </c>
+      <c r="Z28" s="45">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AA28" s="47">
+      <c r="AA28" s="45">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AB28" s="47">
+      <c r="AB28" s="45">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AC28" s="47">
+      <c r="AC28" s="45">
         <f>COUNTIF(Table11[[#This Row],[C]:[M]],"&lt;=FILL THIS IN")</f>
         <v>0</v>
       </c>
-      <c r="AD28" s="60">
+      <c r="AD28" s="58">
         <f>SUMIF(Table11[[#This Row],[C]:[M]],"&lt;=FILL THIS IN")</f>
         <v>0</v>
       </c>
-      <c r="AE28" s="61">
+      <c r="AE28" s="59">
         <f t="shared" ref="AE28:AE33" si="3">SUM(Y28:AD28)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF28" s="18">
         <v>5</v>
@@ -4735,98 +4747,100 @@
     </row>
     <row r="29" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A29" s="9">
-        <v>113</v>
+        <v>23</v>
       </c>
       <c r="B29" s="10">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C29" s="10">
         <v>5</v>
       </c>
       <c r="D29" s="10">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="E29" s="10">
+        <v>6</v>
+      </c>
+      <c r="F29" s="10">
         <v>3</v>
-      </c>
-      <c r="F29" s="10">
-        <v>5</v>
       </c>
       <c r="G29" s="10"/>
       <c r="H29" s="10"/>
       <c r="I29" s="10"/>
       <c r="J29" s="11"/>
-      <c r="K29" s="19">
+      <c r="K29" s="54">
         <f>COUNTIF(Table5[[#This Row],[A]:[E]], 1)</f>
+        <v>0</v>
+      </c>
+      <c r="L29" s="55">
+        <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=2")</f>
+        <v>0</v>
+      </c>
+      <c r="M29" s="55">
+        <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=3")</f>
         <v>1</v>
       </c>
-      <c r="L29" s="20">
-        <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=2")</f>
+      <c r="N29" s="55">
+        <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=4")</f>
+        <v>1</v>
+      </c>
+      <c r="O29" s="55">
+        <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=5")</f>
         <v>2</v>
       </c>
-      <c r="M29" s="20">
-        <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=3")</f>
-        <v>3</v>
-      </c>
-      <c r="N29" s="20">
-        <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=4")</f>
-        <v>3</v>
-      </c>
-      <c r="O29" s="20">
-        <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=5")</f>
-        <v>5</v>
-      </c>
-      <c r="P29" s="20">
+      <c r="P29" s="55">
         <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=6")</f>
-        <v>5</v>
-      </c>
-      <c r="Q29" s="20">
+        <v>4</v>
+      </c>
+      <c r="Q29" s="55">
         <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=7")</f>
         <v>5</v>
       </c>
-      <c r="R29" s="20">
+      <c r="R29" s="55">
         <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=8")</f>
         <v>5</v>
       </c>
-      <c r="S29" s="20">
-        <f>SUMIF(Table5[[#This Row],[A]:[E]],"&lt;=FILL THIS IN")</f>
-        <v>0</v>
-      </c>
-      <c r="T29" s="20">
-        <f>SUMIF(Table5[[#This Row],[A]:[E]],"&lt;=FILL THIS IN")</f>
-        <v>0</v>
-      </c>
-      <c r="U29" s="33"/>
-      <c r="V29" s="21"/>
-      <c r="X29" s="49">
+      <c r="S29" s="55">
+        <f>SUMIF(Table5[[#This Row],[A]:[E]],"&lt;=2")</f>
+        <v>0</v>
+      </c>
+      <c r="T29" s="55">
+        <f>SUMIF(Table5[[#This Row],[A]:[E]],"&lt;=3")</f>
+        <v>3</v>
+      </c>
+      <c r="U29" s="56"/>
+      <c r="V29" s="57" t="s">
+        <v>44</v>
+      </c>
+      <c r="X29" s="47">
         <f>Table5[[#This Row],[No. ]]</f>
-        <v>113</v>
-      </c>
-      <c r="Y29" s="46">
+        <v>23</v>
+      </c>
+      <c r="Y29" s="44" t="str">
         <f>Table5[[#This Row],[Result]]</f>
-        <v>0</v>
-      </c>
-      <c r="Z29" s="47">
+        <v>Tied 4</v>
+      </c>
+      <c r="Z29" s="45">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AA29" s="47">
+      <c r="AA29" s="45">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AB29" s="47">
+      <c r="AB29" s="45">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AC29" s="47">
+      <c r="AC29" s="45">
         <f>COUNTIF(Table11[[#This Row],[C]:[M]],"&lt;=FILL THIS IN")</f>
         <v>0</v>
       </c>
-      <c r="AD29" s="60">
+      <c r="AD29" s="58">
         <f>SUMIF(Table11[[#This Row],[C]:[M]],"&lt;=FILL THIS IN")</f>
         <v>0</v>
       </c>
-      <c r="AE29" s="61">
+      <c r="AE29" s="59">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -4836,19 +4850,19 @@
     </row>
     <row r="30" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A30" s="9">
-        <v>114</v>
+        <v>24</v>
       </c>
       <c r="B30" s="10">
+        <v>2</v>
+      </c>
+      <c r="C30" s="10">
+        <v>2</v>
+      </c>
+      <c r="D30" s="10">
         <v>3</v>
       </c>
-      <c r="C30" s="10">
-        <v>3</v>
-      </c>
-      <c r="D30" s="10">
+      <c r="E30" s="10">
         <v>4</v>
-      </c>
-      <c r="E30" s="10">
-        <v>5</v>
       </c>
       <c r="F30" s="10">
         <v>1</v>
@@ -4857,77 +4871,79 @@
       <c r="H30" s="10"/>
       <c r="I30" s="10"/>
       <c r="J30" s="11"/>
-      <c r="K30" s="19">
+      <c r="K30" s="54">
         <f>COUNTIF(Table5[[#This Row],[A]:[E]], 1)</f>
         <v>1</v>
       </c>
-      <c r="L30" s="20">
+      <c r="L30" s="55">
         <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=2")</f>
-        <v>1</v>
-      </c>
-      <c r="M30" s="20">
+        <v>3</v>
+      </c>
+      <c r="M30" s="55">
         <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=3")</f>
-        <v>3</v>
-      </c>
-      <c r="N30" s="20">
+        <v>4</v>
+      </c>
+      <c r="N30" s="55">
         <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=4")</f>
-        <v>4</v>
-      </c>
-      <c r="O30" s="20">
+        <v>5</v>
+      </c>
+      <c r="O30" s="55">
         <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=5")</f>
         <v>5</v>
       </c>
-      <c r="P30" s="20">
+      <c r="P30" s="55">
         <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=6")</f>
         <v>5</v>
       </c>
-      <c r="Q30" s="20">
+      <c r="Q30" s="55">
         <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=7")</f>
         <v>5</v>
       </c>
-      <c r="R30" s="20">
+      <c r="R30" s="55">
         <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=8")</f>
         <v>5</v>
       </c>
-      <c r="S30" s="20">
-        <f>SUMIF(Table5[[#This Row],[A]:[E]],"&lt;=FILL THIS IN")</f>
-        <v>0</v>
-      </c>
-      <c r="T30" s="20">
-        <f>SUMIF(Table5[[#This Row],[A]:[E]],"&lt;=FILL THIS IN")</f>
-        <v>0</v>
-      </c>
-      <c r="U30" s="33"/>
-      <c r="V30" s="21"/>
-      <c r="X30" s="49">
+      <c r="S30" s="55">
+        <f>SUMIF(Table5[[#This Row],[A]:[E]],"&lt;=2")</f>
+        <v>5</v>
+      </c>
+      <c r="T30" s="55">
+        <f>SUMIF(Table5[[#This Row],[A]:[E]],"&lt;=3")</f>
+        <v>8</v>
+      </c>
+      <c r="U30" s="56"/>
+      <c r="V30" s="57" t="s">
+        <v>43</v>
+      </c>
+      <c r="X30" s="47">
         <f>Table5[[#This Row],[No. ]]</f>
-        <v>114</v>
-      </c>
-      <c r="Y30" s="46">
+        <v>24</v>
+      </c>
+      <c r="Y30" s="44" t="str">
         <f>Table5[[#This Row],[Result]]</f>
-        <v>0</v>
-      </c>
-      <c r="Z30" s="47">
+        <v>Tied 2</v>
+      </c>
+      <c r="Z30" s="45">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AA30" s="47">
+      <c r="AA30" s="45">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AB30" s="47">
+      <c r="AB30" s="45">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AC30" s="47">
+      <c r="AC30" s="45">
         <f>COUNTIF(Table11[[#This Row],[C]:[M]],"&lt;=FILL THIS IN")</f>
         <v>0</v>
       </c>
-      <c r="AD30" s="60">
+      <c r="AD30" s="58">
         <f>SUMIF(Table11[[#This Row],[C]:[M]],"&lt;=FILL THIS IN")</f>
         <v>0</v>
       </c>
-      <c r="AE30" s="61">
+      <c r="AE30" s="59">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -4937,98 +4953,102 @@
     </row>
     <row r="31" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A31" s="9">
-        <v>115</v>
+        <v>25</v>
       </c>
       <c r="B31" s="10">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C31" s="10">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D31" s="10">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E31" s="10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F31" s="10">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G31" s="10"/>
       <c r="H31" s="10"/>
       <c r="I31" s="10"/>
       <c r="J31" s="11"/>
-      <c r="K31" s="22">
+      <c r="K31" s="86">
         <f>COUNTIF(Table5[[#This Row],[A]:[E]], 1)</f>
+        <v>0</v>
+      </c>
+      <c r="L31" s="87">
+        <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=2")</f>
+        <v>0</v>
+      </c>
+      <c r="M31" s="87">
+        <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=3")</f>
+        <v>1</v>
+      </c>
+      <c r="N31" s="87">
+        <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=4")</f>
         <v>2</v>
       </c>
-      <c r="L31" s="23">
-        <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=2")</f>
-        <v>5</v>
-      </c>
-      <c r="M31" s="23">
-        <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=3")</f>
-        <v>5</v>
-      </c>
-      <c r="N31" s="23">
-        <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=4")</f>
-        <v>5</v>
-      </c>
-      <c r="O31" s="23">
+      <c r="O31" s="87">
         <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=5")</f>
-        <v>5</v>
-      </c>
-      <c r="P31" s="23">
+        <v>4</v>
+      </c>
+      <c r="P31" s="87">
         <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=6")</f>
         <v>5</v>
       </c>
-      <c r="Q31" s="23">
+      <c r="Q31" s="87">
         <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=7")</f>
         <v>5</v>
       </c>
-      <c r="R31" s="23">
+      <c r="R31" s="87">
         <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=8")</f>
         <v>5</v>
       </c>
-      <c r="S31" s="23">
-        <f>SUMIF(Table5[[#This Row],[A]:[E]],"&lt;=FILL THIS IN")</f>
-        <v>0</v>
-      </c>
-      <c r="T31" s="23">
-        <f>SUMIF(Table5[[#This Row],[A]:[E]],"&lt;=FILL THIS IN")</f>
-        <v>0</v>
-      </c>
-      <c r="U31" s="34"/>
-      <c r="V31" s="24"/>
-      <c r="X31" s="49">
+      <c r="S31" s="87">
+        <f>SUMIF(Table5[[#This Row],[A]:[E]],"&lt;=2")</f>
+        <v>0</v>
+      </c>
+      <c r="T31" s="87">
+        <f>SUMIF(Table5[[#This Row],[A]:[E]],"&lt;=3")</f>
+        <v>3</v>
+      </c>
+      <c r="U31" s="88" t="s">
+        <v>24</v>
+      </c>
+      <c r="V31" s="89" t="s">
+        <v>44</v>
+      </c>
+      <c r="X31" s="47">
         <f>Table5[[#This Row],[No. ]]</f>
-        <v>115</v>
-      </c>
-      <c r="Y31" s="46">
+        <v>25</v>
+      </c>
+      <c r="Y31" s="44" t="str">
         <f>Table5[[#This Row],[Result]]</f>
-        <v>0</v>
-      </c>
-      <c r="Z31" s="47">
+        <v>Tied 4</v>
+      </c>
+      <c r="Z31" s="45">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AA31" s="47">
+      <c r="AA31" s="45">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AB31" s="47">
+      <c r="AB31" s="45">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AC31" s="47">
+      <c r="AC31" s="45">
         <f>COUNTIF(Table11[[#This Row],[C]:[M]],"&lt;=FILL THIS IN")</f>
         <v>0</v>
       </c>
-      <c r="AD31" s="60">
+      <c r="AD31" s="58">
         <f>SUMIF(Table11[[#This Row],[C]:[M]],"&lt;=FILL THIS IN")</f>
         <v>0</v>
       </c>
-      <c r="AE31" s="61">
+      <c r="AE31" s="59">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -5038,98 +5058,100 @@
     </row>
     <row r="32" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A32" s="9">
-        <v>116</v>
+        <v>26</v>
       </c>
       <c r="B32" s="10">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C32" s="10">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D32" s="10">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E32" s="10">
         <v>1</v>
       </c>
       <c r="F32" s="10">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G32" s="10"/>
       <c r="H32" s="10"/>
       <c r="I32" s="10"/>
       <c r="J32" s="11"/>
-      <c r="K32" s="19">
+      <c r="K32" s="54">
         <f>COUNTIF(Table5[[#This Row],[A]:[E]], 1)</f>
         <v>1</v>
       </c>
-      <c r="L32" s="20">
+      <c r="L32" s="55">
         <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=2")</f>
-        <v>1</v>
-      </c>
-      <c r="M32" s="20">
+        <v>3</v>
+      </c>
+      <c r="M32" s="55">
         <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=3")</f>
-        <v>2</v>
-      </c>
-      <c r="N32" s="20">
+        <v>4</v>
+      </c>
+      <c r="N32" s="55">
         <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=4")</f>
-        <v>3</v>
-      </c>
-      <c r="O32" s="20">
+        <v>5</v>
+      </c>
+      <c r="O32" s="55">
         <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=5")</f>
-        <v>4</v>
-      </c>
-      <c r="P32" s="20">
+        <v>5</v>
+      </c>
+      <c r="P32" s="55">
         <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=6")</f>
         <v>5</v>
       </c>
-      <c r="Q32" s="20">
+      <c r="Q32" s="55">
         <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=7")</f>
         <v>5</v>
       </c>
-      <c r="R32" s="20">
+      <c r="R32" s="55">
         <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=8")</f>
         <v>5</v>
       </c>
-      <c r="S32" s="20">
-        <f>SUMIF(Table5[[#This Row],[A]:[E]],"&lt;=FILL THIS IN")</f>
-        <v>0</v>
-      </c>
-      <c r="T32" s="20">
-        <f>SUMIF(Table5[[#This Row],[A]:[E]],"&lt;=FILL THIS IN")</f>
-        <v>0</v>
-      </c>
-      <c r="U32" s="33"/>
-      <c r="V32" s="21"/>
-      <c r="X32" s="49">
+      <c r="S32" s="55">
+        <f>SUMIF(Table5[[#This Row],[A]:[E]],"&lt;=2")</f>
+        <v>5</v>
+      </c>
+      <c r="T32" s="55">
+        <f>SUMIF(Table5[[#This Row],[A]:[E]],"&lt;=3")</f>
+        <v>8</v>
+      </c>
+      <c r="U32" s="56"/>
+      <c r="V32" s="57" t="s">
+        <v>43</v>
+      </c>
+      <c r="X32" s="47">
         <f>Table5[[#This Row],[No. ]]</f>
-        <v>116</v>
-      </c>
-      <c r="Y32" s="46">
+        <v>26</v>
+      </c>
+      <c r="Y32" s="44" t="str">
         <f>Table5[[#This Row],[Result]]</f>
-        <v>0</v>
-      </c>
-      <c r="Z32" s="47">
+        <v>Tied 2</v>
+      </c>
+      <c r="Z32" s="45">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AA32" s="47">
+      <c r="AA32" s="45">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AB32" s="47">
+      <c r="AB32" s="45">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AC32" s="47">
+      <c r="AC32" s="45">
         <f>COUNTIF(Table11[[#This Row],[C]:[M]],"&lt;=FILL THIS IN")</f>
         <v>0</v>
       </c>
-      <c r="AD32" s="60">
+      <c r="AD32" s="58">
         <f>SUMIF(Table11[[#This Row],[C]:[M]],"&lt;=FILL THIS IN")</f>
         <v>0</v>
       </c>
-      <c r="AE32" s="61">
+      <c r="AE32" s="59">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -5139,100 +5161,102 @@
     </row>
     <row r="33" spans="1:32" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="12">
-        <v>117</v>
+        <v>27</v>
       </c>
       <c r="B33" s="13">
+        <v>3</v>
+      </c>
+      <c r="C33" s="13">
+        <v>4</v>
+      </c>
+      <c r="D33" s="13">
         <v>6</v>
       </c>
-      <c r="C33" s="13">
-        <v>2</v>
-      </c>
-      <c r="D33" s="13">
+      <c r="E33" s="13">
         <v>5</v>
       </c>
-      <c r="E33" s="13">
-        <v>4</v>
-      </c>
       <c r="F33" s="13">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G33" s="13"/>
       <c r="H33" s="13"/>
       <c r="I33" s="13"/>
       <c r="J33" s="14"/>
-      <c r="K33" s="25">
+      <c r="K33" s="23">
         <f>COUNTIF(Table5[[#This Row],[A]:[E]], 1)</f>
         <v>0</v>
       </c>
-      <c r="L33" s="26">
+      <c r="L33" s="24">
         <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=2")</f>
-        <v>1</v>
-      </c>
-      <c r="M33" s="26">
+        <v>0</v>
+      </c>
+      <c r="M33" s="24">
         <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=3")</f>
         <v>1</v>
       </c>
-      <c r="N33" s="26">
+      <c r="N33" s="24">
         <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=4")</f>
         <v>2</v>
       </c>
-      <c r="O33" s="26">
+      <c r="O33" s="24">
         <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=5")</f>
-        <v>3</v>
-      </c>
-      <c r="P33" s="26">
+        <v>4</v>
+      </c>
+      <c r="P33" s="24">
         <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=6")</f>
         <v>5</v>
       </c>
-      <c r="Q33" s="26">
+      <c r="Q33" s="24">
         <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=7")</f>
         <v>5</v>
       </c>
-      <c r="R33" s="26">
+      <c r="R33" s="24">
         <f>COUNTIF(Table5[[#This Row],[A]:[E]],"&lt;=8")</f>
         <v>5</v>
       </c>
-      <c r="S33" s="26">
-        <f>SUMIF(Table5[[#This Row],[A]:[E]],"&lt;=FILL THIS IN")</f>
-        <v>0</v>
-      </c>
-      <c r="T33" s="26">
-        <f>SUMIF(Table5[[#This Row],[A]:[E]],"&lt;=FILL THIS IN")</f>
-        <v>0</v>
-      </c>
-      <c r="U33" s="35"/>
-      <c r="V33" s="27"/>
-      <c r="X33" s="49">
+      <c r="S33" s="24">
+        <f>SUMIF(Table5[[#This Row],[A]:[E]],"&lt;=2")</f>
+        <v>0</v>
+      </c>
+      <c r="T33" s="24">
+        <f>SUMIF(Table5[[#This Row],[A]:[E]],"&lt;=3")</f>
+        <v>3</v>
+      </c>
+      <c r="U33" s="33"/>
+      <c r="V33" s="25">
+        <v>6</v>
+      </c>
+      <c r="X33" s="47">
         <f>Table5[[#This Row],[No. ]]</f>
-        <v>117</v>
-      </c>
-      <c r="Y33" s="46">
+        <v>27</v>
+      </c>
+      <c r="Y33" s="44">
         <f>Table5[[#This Row],[Result]]</f>
-        <v>0</v>
-      </c>
-      <c r="Z33" s="47">
+        <v>6</v>
+      </c>
+      <c r="Z33" s="45">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AA33" s="47">
+      <c r="AA33" s="45">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AB33" s="47">
+      <c r="AB33" s="45">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AC33" s="47">
+      <c r="AC33" s="45">
         <f>COUNTIF(Table11[[#This Row],[C]:[M]],"&lt;=FILL THIS IN")</f>
         <v>0</v>
       </c>
-      <c r="AD33" s="60">
+      <c r="AD33" s="58">
         <f>SUMIF(Table11[[#This Row],[C]:[M]],"&lt;=FILL THIS IN")</f>
         <v>0</v>
       </c>
-      <c r="AE33" s="61">
+      <c r="AE33" s="59">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AF33" s="15">
         <v>6</v>
@@ -5251,29 +5275,29 @@
       <c r="H34" s="76"/>
       <c r="I34" s="76"/>
       <c r="J34" s="77"/>
-      <c r="K34" s="72" t="s">
+      <c r="K34" s="64" t="s">
         <v>18</v>
       </c>
-      <c r="L34" s="73"/>
-      <c r="M34" s="73"/>
-      <c r="N34" s="73"/>
-      <c r="O34" s="73"/>
-      <c r="P34" s="73"/>
-      <c r="Q34" s="73"/>
-      <c r="R34" s="73"/>
-      <c r="S34" s="73"/>
-      <c r="T34" s="73"/>
-      <c r="U34" s="73"/>
-      <c r="V34" s="74"/>
-      <c r="X34" s="50"/>
-      <c r="Y34" s="51"/>
-      <c r="Z34" s="51"/>
-      <c r="AA34" s="51" t="s">
+      <c r="L34" s="65"/>
+      <c r="M34" s="65"/>
+      <c r="N34" s="65"/>
+      <c r="O34" s="65"/>
+      <c r="P34" s="65"/>
+      <c r="Q34" s="65"/>
+      <c r="R34" s="65"/>
+      <c r="S34" s="65"/>
+      <c r="T34" s="65"/>
+      <c r="U34" s="65"/>
+      <c r="V34" s="66"/>
+      <c r="X34" s="48"/>
+      <c r="Y34" s="49"/>
+      <c r="Z34" s="49"/>
+      <c r="AA34" s="49" t="s">
         <v>24</v>
       </c>
-      <c r="AB34" s="51"/>
-      <c r="AC34" s="51"/>
-      <c r="AD34" s="52"/>
+      <c r="AB34" s="49"/>
+      <c r="AC34" s="49"/>
+      <c r="AD34" s="50"/>
       <c r="AE34" s="16"/>
       <c r="AF34" s="16"/>
     </row>
@@ -5308,28 +5332,28 @@
       <c r="J35" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K35" s="40" t="s">
+      <c r="K35" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="L35" s="36" t="s">
+      <c r="L35" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="M35" s="36" t="s">
+      <c r="M35" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="N35" s="36" t="s">
+      <c r="N35" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="O35" s="36" t="s">
+      <c r="O35" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="P35" s="36" t="s">
+      <c r="P35" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="Q35" s="36" t="s">
+      <c r="Q35" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="R35" s="36" t="s">
+      <c r="R35" s="34" t="s">
         <v>17</v>
       </c>
       <c r="S35" s="17" t="s">
@@ -5341,14 +5365,14 @@
       <c r="U35" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="V35" s="41" t="s">
+      <c r="V35" s="39" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="36" spans="1:32" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="5">
         <f t="shared" ref="A36:A42" si="4">A27</f>
-        <v>111</v>
+        <v>21</v>
       </c>
       <c r="B36" s="10"/>
       <c r="C36" s="10"/>
@@ -5391,18 +5415,18 @@
         <f>COUNTIF(Table6[[#This Row],[A]:[E]],"&lt;=8")</f>
         <v>0</v>
       </c>
-      <c r="S36" s="57">
+      <c r="S36" s="55">
         <f>SUMIF(Table6[[#This Row],[A]:[E]],"&lt;=FILL THIS IN")</f>
         <v>0</v>
       </c>
       <c r="T36" s="20"/>
-      <c r="U36" s="33"/>
-      <c r="V36" s="29"/>
+      <c r="U36" s="31"/>
+      <c r="V36" s="27"/>
     </row>
     <row r="37" spans="1:32" ht="19" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A37" s="9">
         <f t="shared" si="4"/>
-        <v>112</v>
+        <v>22</v>
       </c>
       <c r="B37" s="10"/>
       <c r="C37" s="10"/>
@@ -5413,7 +5437,7 @@
       <c r="H37" s="10"/>
       <c r="I37" s="10"/>
       <c r="J37" s="11"/>
-      <c r="K37" s="28">
+      <c r="K37" s="26">
         <f>COUNTIF(Table6[[#This Row],[A]:[E]], 1)</f>
         <v>0</v>
       </c>
@@ -5450,24 +5474,24 @@
         <v>0</v>
       </c>
       <c r="T37" s="20"/>
-      <c r="U37" s="33"/>
-      <c r="V37" s="29"/>
-      <c r="X37" s="83" t="s">
+      <c r="U37" s="31"/>
+      <c r="V37" s="27"/>
+      <c r="X37" s="70" t="s">
         <v>26</v>
       </c>
-      <c r="Y37" s="84"/>
-      <c r="Z37" s="84"/>
-      <c r="AA37" s="84"/>
-      <c r="AB37" s="84"/>
-      <c r="AC37" s="84"/>
-      <c r="AD37" s="84"/>
-      <c r="AE37" s="84"/>
-      <c r="AF37" s="85"/>
+      <c r="Y37" s="71"/>
+      <c r="Z37" s="71"/>
+      <c r="AA37" s="71"/>
+      <c r="AB37" s="71"/>
+      <c r="AC37" s="71"/>
+      <c r="AD37" s="71"/>
+      <c r="AE37" s="71"/>
+      <c r="AF37" s="72"/>
     </row>
     <row r="38" spans="1:32" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="9">
         <f t="shared" si="4"/>
-        <v>113</v>
+        <v>23</v>
       </c>
       <c r="B38" s="10"/>
       <c r="C38" s="10"/>
@@ -5478,7 +5502,7 @@
       <c r="H38" s="10"/>
       <c r="I38" s="10"/>
       <c r="J38" s="11"/>
-      <c r="K38" s="28">
+      <c r="K38" s="26">
         <f>COUNTIF(Table6[[#This Row],[A]:[E]], 1)</f>
         <v>0</v>
       </c>
@@ -5515,26 +5539,26 @@
         <v>0</v>
       </c>
       <c r="T38" s="20"/>
-      <c r="U38" s="33"/>
-      <c r="V38" s="29"/>
-      <c r="X38" s="78" t="s">
+      <c r="U38" s="31"/>
+      <c r="V38" s="27"/>
+      <c r="X38" s="84" t="s">
         <v>35</v>
       </c>
-      <c r="Y38" s="67"/>
-      <c r="Z38" s="67"/>
-      <c r="AA38" s="67"/>
-      <c r="AB38" s="79"/>
-      <c r="AC38" s="66" t="s">
+      <c r="Y38" s="79"/>
+      <c r="Z38" s="79"/>
+      <c r="AA38" s="79"/>
+      <c r="AB38" s="85"/>
+      <c r="AC38" s="78" t="s">
         <v>36</v>
       </c>
-      <c r="AD38" s="67"/>
-      <c r="AE38" s="67"/>
-      <c r="AF38" s="68"/>
+      <c r="AD38" s="79"/>
+      <c r="AE38" s="79"/>
+      <c r="AF38" s="80"/>
     </row>
     <row r="39" spans="1:32" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="9">
         <f t="shared" si="4"/>
-        <v>114</v>
+        <v>24</v>
       </c>
       <c r="B39" s="10"/>
       <c r="C39" s="10"/>
@@ -5545,7 +5569,7 @@
       <c r="H39" s="10"/>
       <c r="I39" s="10"/>
       <c r="J39" s="11"/>
-      <c r="K39" s="28">
+      <c r="K39" s="26">
         <f>COUNTIF(Table6[[#This Row],[A]:[E]], 1)</f>
         <v>0</v>
       </c>
@@ -5582,40 +5606,40 @@
         <v>0</v>
       </c>
       <c r="T39" s="20"/>
-      <c r="U39" s="33"/>
-      <c r="V39" s="29"/>
+      <c r="U39" s="31"/>
+      <c r="V39" s="27"/>
       <c r="X39" s="3" t="s">
         <v>27</v>
       </c>
       <c r="Y39" s="1">
         <v>1</v>
       </c>
-      <c r="Z39" s="65" t="s">
+      <c r="Z39" s="63" t="s">
         <v>11</v>
       </c>
-      <c r="AA39" s="65" t="s">
+      <c r="AA39" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="AB39" s="65" t="s">
+      <c r="AB39" s="63" t="s">
         <v>13</v>
       </c>
-      <c r="AC39" s="65" t="s">
+      <c r="AC39" s="63" t="s">
         <v>14</v>
       </c>
-      <c r="AD39" s="65" t="s">
+      <c r="AD39" s="63" t="s">
         <v>15</v>
       </c>
-      <c r="AE39" s="65" t="s">
+      <c r="AE39" s="63" t="s">
         <v>16</v>
       </c>
-      <c r="AF39" s="55" t="s">
+      <c r="AF39" s="53" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="40" spans="1:32" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A40" s="9">
         <f t="shared" si="4"/>
-        <v>115</v>
+        <v>25</v>
       </c>
       <c r="B40" s="10"/>
       <c r="C40" s="10"/>
@@ -5626,45 +5650,45 @@
       <c r="H40" s="10"/>
       <c r="I40" s="10"/>
       <c r="J40" s="11"/>
-      <c r="K40" s="30">
+      <c r="K40" s="28">
         <f>COUNTIF(Table6[[#This Row],[A]:[E]], 1)</f>
         <v>0</v>
       </c>
-      <c r="L40" s="23">
+      <c r="L40" s="22">
         <f>COUNTIF(Table6[[#This Row],[A]:[E]],"&lt;=2")</f>
         <v>0</v>
       </c>
-      <c r="M40" s="23">
+      <c r="M40" s="22">
         <f>COUNTIF(Table6[[#This Row],[A]:[E]],"&lt;=3")</f>
         <v>0</v>
       </c>
-      <c r="N40" s="23">
+      <c r="N40" s="22">
         <f>COUNTIF(Table6[[#This Row],[A]:[E]],"&lt;=4")</f>
         <v>0</v>
       </c>
-      <c r="O40" s="23">
+      <c r="O40" s="22">
         <f>COUNTIF(Table6[[#This Row],[A]:[E]],"&lt;=5")</f>
         <v>0</v>
       </c>
-      <c r="P40" s="23">
+      <c r="P40" s="22">
         <f>COUNTIF(Table6[[#This Row],[A]:[E]],"&lt;=6")</f>
         <v>0</v>
       </c>
-      <c r="Q40" s="23">
+      <c r="Q40" s="22">
         <f>COUNTIF(Table6[[#This Row],[A]:[E]],"&lt;=7")</f>
         <v>0</v>
       </c>
-      <c r="R40" s="23">
+      <c r="R40" s="22">
         <f>COUNTIF(Table6[[#This Row],[A]:[E]],"&lt;=8")</f>
         <v>0</v>
       </c>
-      <c r="S40" s="23">
+      <c r="S40" s="22">
         <f>SUMIF(Table6[[#This Row],[A]:[E]],"&lt;=FILL THIS IN")</f>
         <v>0</v>
       </c>
-      <c r="T40" s="23"/>
-      <c r="U40" s="34"/>
-      <c r="V40" s="37"/>
+      <c r="T40" s="22"/>
+      <c r="U40" s="32"/>
+      <c r="V40" s="35"/>
       <c r="X40" s="5" t="s">
         <v>41</v>
       </c>
@@ -5703,7 +5727,7 @@
     <row r="41" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A41" s="9">
         <f t="shared" si="4"/>
-        <v>116</v>
+        <v>26</v>
       </c>
       <c r="B41" s="10"/>
       <c r="C41" s="10"/>
@@ -5714,7 +5738,7 @@
       <c r="H41" s="10"/>
       <c r="I41" s="10"/>
       <c r="J41" s="11"/>
-      <c r="K41" s="28">
+      <c r="K41" s="26">
         <f>COUNTIF(Table6[[#This Row],[A]:[E]], 1)</f>
         <v>0</v>
       </c>
@@ -5751,8 +5775,8 @@
         <v>0</v>
       </c>
       <c r="T41" s="20"/>
-      <c r="U41" s="33"/>
-      <c r="V41" s="29"/>
+      <c r="U41" s="31"/>
+      <c r="V41" s="27"/>
       <c r="X41" s="9" t="s">
         <v>42</v>
       </c>
@@ -5791,7 +5815,7 @@
     <row r="42" spans="1:32" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A42" s="12">
         <f t="shared" si="4"/>
-        <v>117</v>
+        <v>27</v>
       </c>
       <c r="B42" s="13"/>
       <c r="C42" s="13"/>
@@ -5802,45 +5826,45 @@
       <c r="H42" s="13"/>
       <c r="I42" s="13"/>
       <c r="J42" s="14"/>
-      <c r="K42" s="31">
+      <c r="K42" s="29">
         <f>COUNTIF(Table6[[#This Row],[A]:[E]], 1)</f>
         <v>0</v>
       </c>
-      <c r="L42" s="32">
+      <c r="L42" s="30">
         <f>COUNTIF(Table6[[#This Row],[A]:[E]],"&lt;=2")</f>
         <v>0</v>
       </c>
-      <c r="M42" s="32">
+      <c r="M42" s="30">
         <f>COUNTIF(Table6[[#This Row],[A]:[E]],"&lt;=3")</f>
         <v>0</v>
       </c>
-      <c r="N42" s="32">
+      <c r="N42" s="30">
         <f>COUNTIF(Table6[[#This Row],[A]:[E]],"&lt;=4")</f>
         <v>0</v>
       </c>
-      <c r="O42" s="32">
+      <c r="O42" s="30">
         <f>COUNTIF(Table6[[#This Row],[A]:[E]],"&lt;=5")</f>
         <v>0</v>
       </c>
-      <c r="P42" s="32">
+      <c r="P42" s="30">
         <f>COUNTIF(Table6[[#This Row],[A]:[E]],"&lt;=6")</f>
         <v>0</v>
       </c>
-      <c r="Q42" s="32">
+      <c r="Q42" s="30">
         <f>COUNTIF(Table6[[#This Row],[A]:[E]],"&lt;=7")</f>
         <v>0</v>
       </c>
-      <c r="R42" s="32">
+      <c r="R42" s="30">
         <f>COUNTIF(Table6[[#This Row],[A]:[E]],"&lt;=8")</f>
         <v>0</v>
       </c>
-      <c r="S42" s="32">
+      <c r="S42" s="30">
         <f>SUMIF(Table6[[#This Row],[A]:[E]],"&lt;=FILL THIS IN")</f>
         <v>0</v>
       </c>
-      <c r="T42" s="32"/>
-      <c r="U42" s="38"/>
-      <c r="V42" s="39"/>
+      <c r="T42" s="30"/>
+      <c r="U42" s="36"/>
+      <c r="V42" s="37"/>
       <c r="X42" s="9"/>
       <c r="Y42" s="10">
         <f t="shared" si="6"/>
@@ -5885,20 +5909,20 @@
       <c r="H43" s="76"/>
       <c r="I43" s="76"/>
       <c r="J43" s="77"/>
-      <c r="K43" s="72" t="s">
+      <c r="K43" s="64" t="s">
         <v>18</v>
       </c>
-      <c r="L43" s="73"/>
-      <c r="M43" s="73"/>
-      <c r="N43" s="73"/>
-      <c r="O43" s="73"/>
-      <c r="P43" s="73"/>
-      <c r="Q43" s="73"/>
-      <c r="R43" s="73"/>
-      <c r="S43" s="73"/>
-      <c r="T43" s="73"/>
-      <c r="U43" s="73"/>
-      <c r="V43" s="74"/>
+      <c r="L43" s="65"/>
+      <c r="M43" s="65"/>
+      <c r="N43" s="65"/>
+      <c r="O43" s="65"/>
+      <c r="P43" s="65"/>
+      <c r="Q43" s="65"/>
+      <c r="R43" s="65"/>
+      <c r="S43" s="65"/>
+      <c r="T43" s="65"/>
+      <c r="U43" s="65"/>
+      <c r="V43" s="66"/>
       <c r="X43" s="9"/>
       <c r="Y43" s="10">
         <f t="shared" si="6"/>
@@ -5961,28 +5985,28 @@
       <c r="J44" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K44" s="40" t="s">
+      <c r="K44" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="L44" s="36" t="s">
+      <c r="L44" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="M44" s="36" t="s">
+      <c r="M44" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="N44" s="36" t="s">
+      <c r="N44" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="O44" s="36" t="s">
+      <c r="O44" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="P44" s="36" t="s">
+      <c r="P44" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="Q44" s="36" t="s">
+      <c r="Q44" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="R44" s="36" t="s">
+      <c r="R44" s="34" t="s">
         <v>17</v>
       </c>
       <c r="S44" s="17" t="s">
@@ -5994,7 +6018,7 @@
       <c r="U44" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="V44" s="42" t="s">
+      <c r="V44" s="40" t="s">
         <v>19</v>
       </c>
       <c r="X44" s="9"/>
@@ -6031,7 +6055,7 @@
     <row r="45" spans="1:32" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A45" s="5">
         <f t="shared" ref="A45:A51" si="7">A27</f>
-        <v>111</v>
+        <v>21</v>
       </c>
       <c r="B45" s="10"/>
       <c r="C45" s="10"/>
@@ -6074,13 +6098,13 @@
         <f>COUNTIF(Table7[[#This Row],[A]:[E]],"&lt;=8")</f>
         <v>0</v>
       </c>
-      <c r="S45" s="57">
+      <c r="S45" s="55">
         <f>SUMIF(Table7[[#This Row],[A]:[E]],"&lt;=FILL THIS IN")</f>
         <v>0</v>
       </c>
       <c r="T45" s="20"/>
-      <c r="U45" s="33"/>
-      <c r="V45" s="29"/>
+      <c r="U45" s="31"/>
+      <c r="V45" s="27"/>
       <c r="X45" s="9"/>
       <c r="Y45" s="10">
         <f t="shared" si="6"/>
@@ -6115,7 +6139,7 @@
     <row r="46" spans="1:32" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A46" s="9">
         <f t="shared" si="7"/>
-        <v>112</v>
+        <v>22</v>
       </c>
       <c r="B46" s="10"/>
       <c r="C46" s="10"/>
@@ -6126,7 +6150,7 @@
       <c r="H46" s="10"/>
       <c r="I46" s="10"/>
       <c r="J46" s="11"/>
-      <c r="K46" s="28">
+      <c r="K46" s="26">
         <f>COUNTIF(Table7[[#This Row],[A]:[E]], 1)</f>
         <v>0</v>
       </c>
@@ -6163,8 +6187,8 @@
         <v>0</v>
       </c>
       <c r="T46" s="20"/>
-      <c r="U46" s="33"/>
-      <c r="V46" s="29"/>
+      <c r="U46" s="31"/>
+      <c r="V46" s="27"/>
       <c r="X46" s="12"/>
       <c r="Y46" s="13"/>
       <c r="Z46" s="13"/>
@@ -6178,7 +6202,7 @@
     <row r="47" spans="1:32" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A47" s="9">
         <f t="shared" si="7"/>
-        <v>113</v>
+        <v>23</v>
       </c>
       <c r="B47" s="10"/>
       <c r="C47" s="10"/>
@@ -6189,7 +6213,7 @@
       <c r="H47" s="10"/>
       <c r="I47" s="10"/>
       <c r="J47" s="11"/>
-      <c r="K47" s="28">
+      <c r="K47" s="26">
         <f>COUNTIF(Table7[[#This Row],[A]:[E]], 1)</f>
         <v>0</v>
       </c>
@@ -6226,13 +6250,13 @@
         <v>0</v>
       </c>
       <c r="T47" s="20"/>
-      <c r="U47" s="33"/>
-      <c r="V47" s="29"/>
+      <c r="U47" s="31"/>
+      <c r="V47" s="27"/>
     </row>
     <row r="48" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A48" s="9">
         <f t="shared" si="7"/>
-        <v>114</v>
+        <v>24</v>
       </c>
       <c r="B48" s="10"/>
       <c r="C48" s="10"/>
@@ -6243,7 +6267,7 @@
       <c r="H48" s="10"/>
       <c r="I48" s="10"/>
       <c r="J48" s="11"/>
-      <c r="K48" s="28">
+      <c r="K48" s="26">
         <f>COUNTIF(Table7[[#This Row],[A]:[E]], 1)</f>
         <v>0</v>
       </c>
@@ -6280,13 +6304,13 @@
         <v>0</v>
       </c>
       <c r="T48" s="20"/>
-      <c r="U48" s="33"/>
-      <c r="V48" s="29"/>
+      <c r="U48" s="31"/>
+      <c r="V48" s="27"/>
     </row>
     <row r="49" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A49" s="9">
         <f t="shared" si="7"/>
-        <v>115</v>
+        <v>25</v>
       </c>
       <c r="B49" s="10"/>
       <c r="C49" s="10"/>
@@ -6297,50 +6321,50 @@
       <c r="H49" s="10"/>
       <c r="I49" s="10"/>
       <c r="J49" s="11"/>
-      <c r="K49" s="30">
+      <c r="K49" s="28">
         <f>COUNTIF(Table7[[#This Row],[A]:[E]], 1)</f>
         <v>0</v>
       </c>
-      <c r="L49" s="23">
+      <c r="L49" s="22">
         <f>COUNTIF(Table7[[#This Row],[A]:[E]],"&lt;=2")</f>
         <v>0</v>
       </c>
-      <c r="M49" s="23">
+      <c r="M49" s="22">
         <f>COUNTIF(Table7[[#This Row],[A]:[E]],"&lt;=3")</f>
         <v>0</v>
       </c>
-      <c r="N49" s="23">
+      <c r="N49" s="22">
         <f>COUNTIF(Table7[[#This Row],[A]:[E]],"&lt;=4")</f>
         <v>0</v>
       </c>
-      <c r="O49" s="23">
+      <c r="O49" s="22">
         <f>COUNTIF(Table7[[#This Row],[A]:[E]],"&lt;=5")</f>
         <v>0</v>
       </c>
-      <c r="P49" s="23">
+      <c r="P49" s="22">
         <f>COUNTIF(Table7[[#This Row],[A]:[E]],"&lt;=6")</f>
         <v>0</v>
       </c>
-      <c r="Q49" s="23">
+      <c r="Q49" s="22">
         <f>COUNTIF(Table7[[#This Row],[A]:[E]],"&lt;=7")</f>
         <v>0</v>
       </c>
-      <c r="R49" s="23">
+      <c r="R49" s="22">
         <f>COUNTIF(Table7[[#This Row],[A]:[E]],"&lt;=8")</f>
         <v>0</v>
       </c>
-      <c r="S49" s="23">
+      <c r="S49" s="22">
         <f>SUMIF(Table7[[#This Row],[A]:[E]],"&lt;=FILL THIS IN")</f>
         <v>0</v>
       </c>
-      <c r="T49" s="23"/>
-      <c r="U49" s="34"/>
-      <c r="V49" s="37"/>
+      <c r="T49" s="22"/>
+      <c r="U49" s="32"/>
+      <c r="V49" s="35"/>
     </row>
     <row r="50" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A50" s="9">
         <f t="shared" si="7"/>
-        <v>116</v>
+        <v>26</v>
       </c>
       <c r="B50" s="10"/>
       <c r="C50" s="10"/>
@@ -6351,7 +6375,7 @@
       <c r="H50" s="10"/>
       <c r="I50" s="10"/>
       <c r="J50" s="11"/>
-      <c r="K50" s="28">
+      <c r="K50" s="26">
         <f>COUNTIF(Table7[[#This Row],[A]:[E]], 1)</f>
         <v>0</v>
       </c>
@@ -6388,13 +6412,13 @@
         <v>0</v>
       </c>
       <c r="T50" s="20"/>
-      <c r="U50" s="33"/>
-      <c r="V50" s="29"/>
+      <c r="U50" s="31"/>
+      <c r="V50" s="27"/>
     </row>
     <row r="51" spans="1:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A51" s="12">
         <f t="shared" si="7"/>
-        <v>117</v>
+        <v>27</v>
       </c>
       <c r="B51" s="13"/>
       <c r="C51" s="13"/>
@@ -6405,73 +6429,73 @@
       <c r="H51" s="13"/>
       <c r="I51" s="13"/>
       <c r="J51" s="14"/>
-      <c r="K51" s="31">
+      <c r="K51" s="29">
         <f>COUNTIF(Table7[[#This Row],[A]:[E]], 1)</f>
         <v>0</v>
       </c>
-      <c r="L51" s="32">
+      <c r="L51" s="30">
         <f>COUNTIF(Table7[[#This Row],[A]:[E]],"&lt;=2")</f>
         <v>0</v>
       </c>
-      <c r="M51" s="32">
+      <c r="M51" s="30">
         <f>COUNTIF(Table7[[#This Row],[A]:[E]],"&lt;=3")</f>
         <v>0</v>
       </c>
-      <c r="N51" s="32">
+      <c r="N51" s="30">
         <f>COUNTIF(Table7[[#This Row],[A]:[E]],"&lt;=4")</f>
         <v>0</v>
       </c>
-      <c r="O51" s="32">
+      <c r="O51" s="30">
         <f>COUNTIF(Table7[[#This Row],[A]:[E]],"&lt;=5")</f>
         <v>0</v>
       </c>
-      <c r="P51" s="32">
+      <c r="P51" s="30">
         <f>COUNTIF(Table7[[#This Row],[A]:[E]],"&lt;=6")</f>
         <v>0</v>
       </c>
-      <c r="Q51" s="32">
+      <c r="Q51" s="30">
         <f>COUNTIF(Table7[[#This Row],[A]:[E]],"&lt;=7")</f>
         <v>0</v>
       </c>
-      <c r="R51" s="32">
+      <c r="R51" s="30">
         <f>COUNTIF(Table7[[#This Row],[A]:[E]],"&lt;=8")</f>
         <v>0</v>
       </c>
-      <c r="S51" s="32">
+      <c r="S51" s="30">
         <f>SUMIF(Table7[[#This Row],[A]:[E]],"&lt;=FILL THIS IN")</f>
         <v>0</v>
       </c>
-      <c r="T51" s="32"/>
-      <c r="U51" s="38"/>
-      <c r="V51" s="39"/>
+      <c r="T51" s="30"/>
+      <c r="U51" s="36"/>
+      <c r="V51" s="37"/>
     </row>
     <row r="52" spans="1:22" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="69" t="s">
+      <c r="A52" s="81" t="s">
         <v>34</v>
       </c>
-      <c r="B52" s="70"/>
-      <c r="C52" s="70"/>
-      <c r="D52" s="70"/>
-      <c r="E52" s="70"/>
-      <c r="F52" s="70"/>
-      <c r="G52" s="70"/>
-      <c r="H52" s="70"/>
-      <c r="I52" s="70"/>
-      <c r="J52" s="71"/>
-      <c r="K52" s="72" t="s">
+      <c r="B52" s="82"/>
+      <c r="C52" s="82"/>
+      <c r="D52" s="82"/>
+      <c r="E52" s="82"/>
+      <c r="F52" s="82"/>
+      <c r="G52" s="82"/>
+      <c r="H52" s="82"/>
+      <c r="I52" s="82"/>
+      <c r="J52" s="83"/>
+      <c r="K52" s="64" t="s">
         <v>18</v>
       </c>
-      <c r="L52" s="73"/>
-      <c r="M52" s="73"/>
-      <c r="N52" s="73"/>
-      <c r="O52" s="73"/>
-      <c r="P52" s="73"/>
-      <c r="Q52" s="73"/>
-      <c r="R52" s="73"/>
-      <c r="S52" s="73"/>
-      <c r="T52" s="73"/>
-      <c r="U52" s="73"/>
-      <c r="V52" s="74"/>
+      <c r="L52" s="65"/>
+      <c r="M52" s="65"/>
+      <c r="N52" s="65"/>
+      <c r="O52" s="65"/>
+      <c r="P52" s="65"/>
+      <c r="Q52" s="65"/>
+      <c r="R52" s="65"/>
+      <c r="S52" s="65"/>
+      <c r="T52" s="65"/>
+      <c r="U52" s="65"/>
+      <c r="V52" s="66"/>
     </row>
     <row r="53" spans="1:22" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
@@ -6504,28 +6528,28 @@
       <c r="J53" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K53" s="40" t="s">
+      <c r="K53" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="L53" s="36" t="s">
+      <c r="L53" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="M53" s="36" t="s">
+      <c r="M53" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="N53" s="36" t="s">
+      <c r="N53" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="O53" s="36" t="s">
+      <c r="O53" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="P53" s="36" t="s">
+      <c r="P53" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="Q53" s="36" t="s">
+      <c r="Q53" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="R53" s="43" t="s">
+      <c r="R53" s="41" t="s">
         <v>17</v>
       </c>
       <c r="S53" s="17" t="s">
@@ -6537,14 +6561,14 @@
       <c r="U53" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="V53" s="41" t="s">
+      <c r="V53" s="39" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="54" spans="1:22" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A54" s="5">
         <f t="shared" ref="A54:A60" si="8">A27</f>
-        <v>111</v>
+        <v>21</v>
       </c>
       <c r="B54" s="10"/>
       <c r="C54" s="10"/>
@@ -6587,18 +6611,18 @@
         <f>COUNTIF(Table8[[#This Row],[A]:[E]],"&lt;=8")</f>
         <v>0</v>
       </c>
-      <c r="S54" s="57">
+      <c r="S54" s="55">
         <f>SUMIF(Table8[[#This Row],[A]:[E]],"&lt;=FILL THIS IN")</f>
         <v>0</v>
       </c>
       <c r="T54" s="20"/>
-      <c r="U54" s="33"/>
-      <c r="V54" s="29"/>
+      <c r="U54" s="31"/>
+      <c r="V54" s="27"/>
     </row>
     <row r="55" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A55" s="9">
         <f t="shared" si="8"/>
-        <v>112</v>
+        <v>22</v>
       </c>
       <c r="B55" s="10"/>
       <c r="C55" s="10"/>
@@ -6609,7 +6633,7 @@
       <c r="H55" s="10"/>
       <c r="I55" s="10"/>
       <c r="J55" s="11"/>
-      <c r="K55" s="28">
+      <c r="K55" s="26">
         <f>COUNTIF(Table8[[#This Row],[A]:[E]], 1)</f>
         <v>0</v>
       </c>
@@ -6646,13 +6670,13 @@
         <v>0</v>
       </c>
       <c r="T55" s="20"/>
-      <c r="U55" s="33"/>
-      <c r="V55" s="29"/>
+      <c r="U55" s="31"/>
+      <c r="V55" s="27"/>
     </row>
     <row r="56" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A56" s="9">
         <f t="shared" si="8"/>
-        <v>113</v>
+        <v>23</v>
       </c>
       <c r="B56" s="10"/>
       <c r="C56" s="10"/>
@@ -6663,7 +6687,7 @@
       <c r="H56" s="10"/>
       <c r="I56" s="10"/>
       <c r="J56" s="11"/>
-      <c r="K56" s="28">
+      <c r="K56" s="26">
         <f>COUNTIF(Table8[[#This Row],[A]:[E]], 1)</f>
         <v>0</v>
       </c>
@@ -6700,13 +6724,13 @@
         <v>0</v>
       </c>
       <c r="T56" s="20"/>
-      <c r="U56" s="33"/>
-      <c r="V56" s="29"/>
+      <c r="U56" s="31"/>
+      <c r="V56" s="27"/>
     </row>
     <row r="57" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A57" s="9">
         <f t="shared" si="8"/>
-        <v>114</v>
+        <v>24</v>
       </c>
       <c r="B57" s="10"/>
       <c r="C57" s="10"/>
@@ -6717,7 +6741,7 @@
       <c r="H57" s="10"/>
       <c r="I57" s="10"/>
       <c r="J57" s="11"/>
-      <c r="K57" s="28">
+      <c r="K57" s="26">
         <f>COUNTIF(Table8[[#This Row],[A]:[E]], 1)</f>
         <v>0</v>
       </c>
@@ -6754,13 +6778,13 @@
         <v>0</v>
       </c>
       <c r="T57" s="20"/>
-      <c r="U57" s="33"/>
-      <c r="V57" s="29"/>
+      <c r="U57" s="31"/>
+      <c r="V57" s="27"/>
     </row>
     <row r="58" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A58" s="9">
         <f t="shared" si="8"/>
-        <v>115</v>
+        <v>25</v>
       </c>
       <c r="B58" s="10"/>
       <c r="C58" s="10"/>
@@ -6771,50 +6795,50 @@
       <c r="H58" s="10"/>
       <c r="I58" s="10"/>
       <c r="J58" s="11"/>
-      <c r="K58" s="30">
+      <c r="K58" s="28">
         <f>COUNTIF(Table8[[#This Row],[A]:[E]], 1)</f>
         <v>0</v>
       </c>
-      <c r="L58" s="23">
+      <c r="L58" s="22">
         <f>COUNTIF(Table8[[#This Row],[A]:[E]],"&lt;=2")</f>
         <v>0</v>
       </c>
-      <c r="M58" s="23">
+      <c r="M58" s="22">
         <f>COUNTIF(Table8[[#This Row],[A]:[E]],"&lt;=3")</f>
         <v>0</v>
       </c>
-      <c r="N58" s="23">
+      <c r="N58" s="22">
         <f>COUNTIF(Table8[[#This Row],[A]:[E]],"&lt;=4")</f>
         <v>0</v>
       </c>
-      <c r="O58" s="23">
+      <c r="O58" s="22">
         <f>COUNTIF(Table8[[#This Row],[A]:[E]],"&lt;=5")</f>
         <v>0</v>
       </c>
-      <c r="P58" s="23">
+      <c r="P58" s="22">
         <f>COUNTIF(Table8[[#This Row],[A]:[E]],"&lt;=6")</f>
         <v>0</v>
       </c>
-      <c r="Q58" s="23">
+      <c r="Q58" s="22">
         <f>COUNTIF(Table8[[#This Row],[A]:[E]],"&lt;=7")</f>
         <v>0</v>
       </c>
-      <c r="R58" s="23">
+      <c r="R58" s="22">
         <f>COUNTIF(Table8[[#This Row],[A]:[E]],"&lt;=8")</f>
         <v>0</v>
       </c>
-      <c r="S58" s="23">
+      <c r="S58" s="22">
         <f>SUMIF(Table8[[#This Row],[A]:[E]],"&lt;=FILL THIS IN")</f>
         <v>0</v>
       </c>
-      <c r="T58" s="23"/>
-      <c r="U58" s="34"/>
-      <c r="V58" s="37"/>
+      <c r="T58" s="22"/>
+      <c r="U58" s="32"/>
+      <c r="V58" s="35"/>
     </row>
     <row r="59" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A59" s="9">
         <f t="shared" si="8"/>
-        <v>116</v>
+        <v>26</v>
       </c>
       <c r="B59" s="10"/>
       <c r="C59" s="10"/>
@@ -6825,7 +6849,7 @@
       <c r="H59" s="10"/>
       <c r="I59" s="10"/>
       <c r="J59" s="11"/>
-      <c r="K59" s="28">
+      <c r="K59" s="26">
         <f>COUNTIF(Table8[[#This Row],[A]:[E]], 1)</f>
         <v>0</v>
       </c>
@@ -6862,13 +6886,13 @@
         <v>0</v>
       </c>
       <c r="T59" s="20"/>
-      <c r="U59" s="33"/>
-      <c r="V59" s="29"/>
+      <c r="U59" s="31"/>
+      <c r="V59" s="27"/>
     </row>
     <row r="60" spans="1:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A60" s="12">
         <f t="shared" si="8"/>
-        <v>117</v>
+        <v>27</v>
       </c>
       <c r="B60" s="13"/>
       <c r="C60" s="13"/>
@@ -6879,61 +6903,61 @@
       <c r="H60" s="13"/>
       <c r="I60" s="13"/>
       <c r="J60" s="14"/>
-      <c r="K60" s="31">
+      <c r="K60" s="29">
         <f>COUNTIF(Table8[[#This Row],[A]:[E]], 1)</f>
         <v>0</v>
       </c>
-      <c r="L60" s="32">
+      <c r="L60" s="30">
         <f>COUNTIF(Table8[[#This Row],[A]:[E]],"&lt;=2")</f>
         <v>0</v>
       </c>
-      <c r="M60" s="32">
+      <c r="M60" s="30">
         <f>COUNTIF(Table8[[#This Row],[A]:[E]],"&lt;=3")</f>
         <v>0</v>
       </c>
-      <c r="N60" s="32">
+      <c r="N60" s="30">
         <f>COUNTIF(Table8[[#This Row],[A]:[E]],"&lt;=4")</f>
         <v>0</v>
       </c>
-      <c r="O60" s="32">
+      <c r="O60" s="30">
         <f>COUNTIF(Table8[[#This Row],[A]:[E]],"&lt;=5")</f>
         <v>0</v>
       </c>
-      <c r="P60" s="32">
+      <c r="P60" s="30">
         <f>COUNTIF(Table8[[#This Row],[A]:[E]],"&lt;=6")</f>
         <v>0</v>
       </c>
-      <c r="Q60" s="32">
+      <c r="Q60" s="30">
         <f>COUNTIF(Table8[[#This Row],[A]:[E]],"&lt;=7")</f>
         <v>0</v>
       </c>
-      <c r="R60" s="32">
+      <c r="R60" s="30">
         <f>COUNTIF(Table8[[#This Row],[A]:[E]],"&lt;=8")</f>
         <v>0</v>
       </c>
-      <c r="S60" s="32">
+      <c r="S60" s="30">
         <f>SUMIF(Table8[[#This Row],[A]:[E]],"&lt;=FILL THIS IN")</f>
         <v>0</v>
       </c>
-      <c r="T60" s="32"/>
-      <c r="U60" s="38"/>
-      <c r="V60" s="39"/>
+      <c r="T60" s="30"/>
+      <c r="U60" s="36"/>
+      <c r="V60" s="37"/>
     </row>
     <row r="61" spans="1:22" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="AC38:AF38"/>
+    <mergeCell ref="A52:J52"/>
+    <mergeCell ref="K52:V52"/>
+    <mergeCell ref="K43:V43"/>
+    <mergeCell ref="A43:J43"/>
+    <mergeCell ref="X38:AB38"/>
     <mergeCell ref="K25:V25"/>
     <mergeCell ref="X25:AF25"/>
     <mergeCell ref="X37:AF37"/>
     <mergeCell ref="A25:J25"/>
     <mergeCell ref="A34:J34"/>
     <mergeCell ref="K34:V34"/>
-    <mergeCell ref="AC38:AF38"/>
-    <mergeCell ref="A52:J52"/>
-    <mergeCell ref="K52:V52"/>
-    <mergeCell ref="K43:V43"/>
-    <mergeCell ref="A43:J43"/>
-    <mergeCell ref="X38:AB38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>